<commit_message>
Handling newline problems: Show newline within td.
</commit_message>
<xml_diff>
--- a/request.xlsx
+++ b/request.xlsx
@@ -247,7 +247,9 @@
     <t>장비개방
 サージュＸシリーズ
 오토모 장비개방
-サージュＸネコブックサージュＸネコフートサージュＸネコスーツ</t>
+サージュＸネコブック_x000D_
+サージュＸネコフート_x000D_
+サージュＸネコスーツ</t>
   </si>
   <si>
     <t>しっかり者の村人の依頼1</t>
@@ -385,7 +387,9 @@
     <t>장비개방
 ホークＸシリーズ
 오토모 장비개방
-ブレイブＸネコランスブレイブＸネコガレアブレイブＸネコロリカ</t>
+ブレイブＸネコランス_x000D_
+ブレイブＸネコガレア_x000D_
+ブレイブＸネコロリカ</t>
   </si>
   <si>
     <t>キャラバンの看板娘の依頼1</t>
@@ -3256,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D190" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E201" sqref="E201"/>
+    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3507,7 +3511,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="60">
+    <row r="15" spans="1:5" ht="90">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -3660,7 +3664,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="60">
+    <row r="24" spans="1:5" ht="90">
       <c r="A24" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
requestQuest: Name translation of equipment and foodstuffs to be opened.(~ベルナ Town)
</commit_message>
<xml_diff>
--- a/request.xlsx
+++ b/request.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19024"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19105"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="781">
   <si>
     <t>town</t>
   </si>
@@ -47,8 +47,8 @@
   </si>
   <si>
     <t>장비개방
-ウィズダムシリーズ
-ウィズダムＸシリーズ</t>
+위즈덤 시리즈(ウィズダムシリーズ)
+위즈덤Ｘ 시리즈(ウィズダムＸシリーズ)</t>
   </si>
   <si>
     <t>龍識船の受付嬢の依頼</t>
@@ -61,11 +61,11 @@
   </si>
   <si>
     <t>장비개방
-チアフルシリーズ_x000D_
-チアフルＸシリーズ
+치어풀 시리즈(チアフルシリーズ)
+치어풀Ｘ 시리즈(チアフルＸシリーズ)
 오토모 장비개방
-チアフルネコフート_x000D_
-チアフルネコスーツ</t>
+치어풀 고양이 후드(チアフルネコフード)
+치어풀 고양이 슈트(チアフルネコスーツ)</t>
   </si>
   <si>
     <t>タンジアの大会担当の依頼</t>
@@ -78,9 +78,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-太古の注連縄
+태고의 금줄(太古の注連縄)
 장비개방
-夜叉/修羅シリーズ</t>
+야차/수라 시리즈(夜叉/修羅シリーズ)</t>
   </si>
   <si>
     <t>モガの農場アイルーの依頼</t>
@@ -92,8 +92,8 @@
     <t>마을★8 진비료를 손에 넣는거다냐!(珍肥料を手に入れるのニャ！)</t>
   </si>
   <si>
-    <t>식재_x000D_
-砲丸レタス</t>
+    <t>식재
+포환 양상추(砲丸レタス)</t>
   </si>
   <si>
     <t>タルアイルーの依頼</t>
@@ -106,11 +106,11 @@
   </si>
   <si>
     <t>식재
-ポッカウォッカ
+폿카 보드카(ポッカウォッカ)
 퀘스트 보수
-タル用特製木材
+나무통용 특제 목재(タル用特製木材)
 오토모장비개방
-タルネコボディ</t>
+나무통 고양이 바디(タルネコボディ)</t>
   </si>
   <si>
     <t>狩猟船団・赤槍の依頼1</t>
@@ -122,8 +122,8 @@
     <t>마을★9 하늘의 가족・밥을 만들겠습니다(空の家族・メシを作るッス)</t>
   </si>
   <si>
-    <t>식재_x000D_
-珍味・甲冑魚</t>
+    <t>식재
+진미・갑주어(珍味・甲冑魚)</t>
   </si>
   <si>
     <t>狩猟船団・赤槍の依頼2</t>
@@ -136,8 +136,8 @@
   </si>
   <si>
     <t>수기개방
-妖刀羅刹LV2
-射突型裂孔弾LV2</t>
+요도나찰LV2(妖刀羅刹LV2)
+사돌형열공탄LV2(射突型裂孔弾LV2)</t>
   </si>
   <si>
     <t>タンジアの銅鑼担当の依頼1</t>
@@ -150,11 +150,11 @@
   </si>
   <si>
     <t>장비개방
-マリネロシリーズ_x000D_
-マリネロＸシリーズ
+마리네로 시리즈(マリネロシリーズ)
+마리네로Ｘ 시리즈(マリネロＸシリーズ)
 오토모 장비개방
-マリネロネコフード_x000D_
-マリネロネコスーツ</t>
+마리네로 고양이 후드(マリネロネコフード)
+마리네로 고양이 슈트(マリネロネコスーツ)</t>
   </si>
   <si>
     <t>タンジアの銅鑼担当の依頼2</t>
@@ -166,9 +166,9 @@
     <t>G★2 ......원한다면 자격을 보여라(……欲するならば資格を示して)</t>
   </si>
   <si>
-    <t>수기개방_x000D_
-インパクトプルスLV2
-アニマートハイLV2</t>
+    <t>수기개방
+임팩트 펄스LV2(インパクトプルスLV2)
+아니마토 하이LV2(アニマートハイLV2)</t>
   </si>
   <si>
     <t>ベルナ村の村長の依頼</t>
@@ -181,11 +181,11 @@
   </si>
   <si>
     <t>장비개방
-龍歴士Ｘシリーズ
+용역사Ｘ 시리즈(龍歴士Ｘシリーズ)
 오토모 장비개방
-エーデルＸネコロッド_x000D_
-エーデルＸネコツイン_x000D_
-エーデルＸネコフリル</t>
+에델Ｘ 고양이 로드(エーデルＸネコロッド)
+에델Ｘ 고양이 트윈(エーデルＸネコツイン)
+에델Ｘ 고양이 프릴(エーデルＸネコフリル)</t>
   </si>
   <si>
     <t>ベルナ村の受付嬢の依頼1</t>
@@ -198,11 +198,11 @@
   </si>
   <si>
     <t>장비개방
-サージュシリーズ
+사쥬 시리즈(サージュシリーズ)
 오토모 장비개방
-サージュネコブック_x000D_
-サージュネコフート_x000D_
-サージュネコスーツ</t>
+사쥬 고양이 책(サージュネコブック)
+사쥬 고양이 후드(サージュネコフード)
+사쥬 고양이 슈트(サージュネコスーツ)</t>
   </si>
   <si>
     <t>ベルナ村の受付嬢の依頼2</t>
@@ -214,8 +214,8 @@
     <t>마을★4 특별한 고비차 만들기(とびきりのゼンマイティー作り)</t>
   </si>
   <si>
-    <t>식재_x000D_
-ゼンマイ米</t>
+    <t>식재
+고비 쌀(ゼンマイ米)</t>
   </si>
   <si>
     <t>ベルナ村の受付嬢の依頼3</t>
@@ -228,11 +228,11 @@
   </si>
   <si>
     <t>장비개방
-サージュSシリーズ
+사쥬Ｓ 시리즈(サージュＳシリーズ)
 오토모 장비개방
-サージュＳネコブック_x000D_
-サージュＳネコフート_x000D_
-サージュＳネコスーツ</t>
+사쥬Ｓ 고양이 책(サージュＳネコブック)
+사쥬Ｓ 고양이 후드(サージュＳネコフード)
+사쥬Ｓ 고양이 슈트(サージュＳネコスーツ)</t>
   </si>
   <si>
     <t>ベルナ村の受付嬢の依頼4</t>
@@ -245,11 +245,11 @@
   </si>
   <si>
     <t>장비개방
-サージュＸシリーズ
+사쥬Ｘ 시리즈(サージュＸシリーズ)
 오토모 장비개방
-サージュＸネコブック_x000D_
-サージュＸネコフート_x000D_
-サージュＸネコスーツ</t>
+사쥬Ｘ 고양이 책(サージュＸネコブック)
+사쥬Ｘ 고양이 후드(サージュＸネコフード)
+사쥬Ｘ 고양이 슈트(サージュＸネコスーツ)</t>
   </si>
   <si>
     <t>しっかり者の村人の依頼1</t>
@@ -262,9 +262,9 @@
   </si>
   <si>
     <t>입수
-星見の花 x1
+성견의 꽃x1 (星見の花 x1)
 퀘스트 보수
-星見の花</t>
+성견의 꽃(星見の花)</t>
   </si>
   <si>
     <t>しっかり者の村人の依頼2</t>
@@ -276,8 +276,8 @@
     <t>마을★3 무파들의 폭신폭신 털뭉치(ムーファたちのふんわり毛玉)</t>
   </si>
   <si>
-    <t>입수_x000D_
-歴院ポイント500pts</t>
+    <t>입수
+용역원 포인트 500pts(龍歴院ポイント500pts)</t>
   </si>
   <si>
     <t>しっかり者の村人の依頼3</t>
@@ -290,7 +290,7 @@
   </si>
   <si>
     <t>장비개방
-龍歴士シリーズ</t>
+용역사 시리즈(龍歴士シリーズ)</t>
   </si>
   <si>
     <t>チコ村の村長の依頼1</t>
@@ -303,7 +303,7 @@
   </si>
   <si>
     <t>장비개방
-しろねこスタンプ</t>
+하얀 고양이 스탬프(しろねこスタンプ)</t>
   </si>
   <si>
     <t>チコ村の村長の依頼2</t>
@@ -316,8 +316,8 @@
   </si>
   <si>
     <t>장비개방
-アイルーラグドール_x000D_
-メラルーラグドール</t>
+아이루 래그돌(アイルーラグドール)
+메라루 래그돌(メラルーラグドール)</t>
   </si>
   <si>
     <t>キャラバンの団長の依頼1</t>
@@ -330,13 +330,13 @@
   </si>
   <si>
     <t>장비개방
-ブレイブシリーズ
+브레이브 시리즈(ブレイブシリーズ)
 오토모 장비개방
-ブレイブネコランス
-ブレイブネコガレア
-ブレイブネコロリカ
-푸기의 옷_x000D_
-夢追いアミーゴ</t>
+브레이브 고양이 랜스(ブレイブネコランス)
+브레이브 고양이 가레아(ブレイブネコガレア)
+브레이브 고양이 로리카(ブレイブネコロリカ)
+푸기의 옷
+꿈을 쫓는 아미고(夢追いアミーゴ)</t>
   </si>
   <si>
     <t>キャラバンの団長の依頼2</t>
@@ -349,12 +349,12 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX天廻龍チケット
+EX천회룡 티켓(EX天廻龍チケット)
 장비개방
-イサナ船ハンマー！_x000D_
-ホークシリーズ_x000D_
-団長の腕輪_x000D_
-団長の腕輪Ｘ</t>
+이사나선 해머!イサナ船ハンマー！
+호크 시리즈(ホークシリーズ)
+단장의 팔찌(団長の腕輪)
+단장의 팔찌Ｘ(団長の腕輪Ｘ)</t>
   </si>
   <si>
     <t>キャラバンの団長の依頼3</t>
@@ -367,12 +367,12 @@
   </si>
   <si>
     <t>장비개방
-ブレイブSシリーズ_x000D_
-ブレイブＸシリーズ
+브레이브Ｓ 시리즈(ブレイブＳシリーズ)
+브레이브Ｘ 시리즈(ブレイブＸシリーズ)
 오토모 장비개방
-ブレイブＳネコランス_x000D_
-ブレイブＳネコガレア_x000D_
-ブレイブＳネコロリカ</t>
+브레이브Ｓ 고양이 랜스(ブレイブＳネコランス)
+브레이브Ｓ 고양이 가레아(ブレイブＳネコガレア)
+브레이브Ｓ 고양이 로리카(ブレイブＳネコロリカ)</t>
   </si>
   <si>
     <t>キャラバンの団長の依頼4</t>
@@ -385,11 +385,11 @@
   </si>
   <si>
     <t>장비개방
-ホークＸシリーズ
+호크Ｘ 시리즈(ホークＸシリーズ)
 오토모 장비개방
-ブレイブＸネコランス_x000D_
-ブレイブＸネコガレア_x000D_
-ブレイブＸネコロリカ</t>
+브레이브Ｘ 고양이 랜스(ブレイブＸネコランス)
+브레이브Ｘ 고양이 가레아(ブレイブＸネコガレア)
+브레이브Ｘ 고양이 로리카(ブレイブＸネコロリカ)</t>
   </si>
   <si>
     <t>キャラバンの看板娘の依頼1</t>
@@ -402,12 +402,12 @@
   </si>
   <si>
     <t>장비개방
-エコールシリーズ
+에콜 시리즈(エコールシリーズ)
 오토모 장비개방
-エコールネコフード
-エコールネコスーツ
+에콜 고양이 후드(エコールネコフード)
+에콜 고양이 슈트(エコールネコスーツ)
 푸기의 옷
-いやされムーチョ</t>
+치유받는무쵸いやされムーチョ</t>
   </si>
   <si>
     <t>キャラバンの看板娘の依頼2</t>
@@ -420,8 +420,8 @@
   </si>
   <si>
     <t>장비개방
-知略の眼鏡_x000D_
-知略の眼鏡Ｘ</t>
+지략의 안경(知略の眼鏡)
+지략의 안경Ｘ(知略の眼鏡Ｘ)</t>
   </si>
   <si>
     <t>キャラバンの看板娘の依頼3</t>
@@ -433,7 +433,7 @@
     <t>집회소★7 초☆메모장 ~천인룡포획편~(超☆メモ帳～千刃竜捕獲編～)</t>
   </si>
   <si>
-    <t>ルームサービス変更可能</t>
+    <t>룸서비스 변경가능(ルームサービス変更可能)</t>
   </si>
   <si>
     <t>キャラバンの看板娘の依頼4</t>
@@ -446,10 +446,10 @@
   </si>
   <si>
     <t>장비개방
-エコールＸシリーズ
+에콜Ｘ 시리즈(エコールＸシリーズ)
 오토모 장비개방
-エコールＸネコフード_x000D_
-エコールＸネコスーツ</t>
+에콜Ｘ 고양이 후드(エコールＸネコフード)
+에콜Ｘ 고양이 슈트(エコールＸネコスーツ)</t>
   </si>
   <si>
     <t>筆頭リーダーの依頼1</t>
@@ -462,9 +462,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX黒蝕竜チケット
+EX흑식룡 티켓(EX黒蝕竜チケット)
 수기개방
-狂竜身(共通)</t>
+광룡신(공통)(狂竜身(共通))</t>
   </si>
   <si>
     <t>筆頭リーダーの依頼2</t>
@@ -477,8 +477,8 @@
   </si>
   <si>
     <t>장비개방
-エースシリーズ_x000D_
-クイーンシリーズ</t>
+에스 시리즈(エースシリーズ)
+퀸 시리즈(クイーンシリーズ)</t>
   </si>
   <si>
     <t>筆頭リーダーの依頼3</t>
@@ -490,9 +490,9 @@
     <t>G★2 밀림의 나르가쿠르가와 대치해라(密林のナルガクルガと対峙せよ)</t>
   </si>
   <si>
-    <t>수기개방_x000D_
-混沌の刃薬LV2
-ラセンザンLV2</t>
+    <t>수기개방
+혼돈의 인약LV2(混沌の刃薬LV2)
+나선참LV2(ラセンザンLV2)</t>
   </si>
   <si>
     <t>筆頭リーダーの依頼4</t>
@@ -505,12 +505,12 @@
   </si>
   <si>
     <t>퀘스트 보수
-混濁した欠片
+혼탁한 조각(混濁した欠片)
 장비개방
-ザッツオール_x000D_
-ウェル_x000D_
-エースＸシリーズ_x000D_
-クイーンＸシリーズ</t>
+That's all(ザッツオール)
+웰(ウェル)
+에스Ｘ 시리즈(エースＸシリーズ)
+퀸Ｘ 시리즈(クイーンＸシリーズ)</t>
   </si>
   <si>
     <t>筆頭ランサーの依頼1</t>
@@ -523,8 +523,8 @@
   </si>
   <si>
     <t>수기개방
-治癒の盾LV2
-AAフレアLV2</t>
+치유의 방패LV2(治癒の盾LV2)
+AA플레어LV2(AAフレアLV2)</t>
   </si>
   <si>
     <t>筆頭ランサーの依頼2</t>
@@ -537,9 +537,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-蝕まれた琥珀
+침식된 호박(蝕まれた琥珀)
 장비개방
-ハイハロウ</t>
+하이하로우(ハイハロウ)</t>
   </si>
   <si>
     <t>筆頭ルーキーの依頼1</t>
@@ -552,13 +552,13 @@
   </si>
   <si>
     <t>퀘스트 보수
-虹色鉱石
+무지개빛 광석(虹色鉱石)
 장비개방
-EXイーオスシリーズ_x000D_
-EXゲネポスシリーズ_x000D_
-EXタロスシリーズ_x000D_
-EXガレオスシリーズ_x000D_
-EXランゴシリーズ</t>
+EX이오스 시리즈(EXイーオスシリーズ)
+EX게네포스 시리즈(EXゲネポスシリーズ)
+EX타로스 시리즈(EXタロスシリーズ)
+EX가레오스 시리즈(EXガレオスシリーズ)
+EX랑고 시리즈(EXランゴシリーズ)</t>
   </si>
   <si>
     <t>筆頭ルーキーの依頼2</t>
@@ -571,8 +571,8 @@
   </si>
   <si>
     <t>수기개방
-テンペストアクスLV2
-チェインソーサーLV2</t>
+템페스트 액스LV2(テンペストアクスLV2)
+체인 소서LV2(チェインソーサーLV2)</t>
   </si>
   <si>
     <t>大老殿の大臣の依頼</t>
@@ -585,12 +585,12 @@
   </si>
   <si>
     <t>장비개방
-ガーディアンＸシリーズ_x000D_
-ガーディアンＺシリーズ
+가디언Ｘ 시리즈(ガーディアンＸシリーズ)
+가디언Ｚ 시리즈(ガーディアンＺシリーズ)
 오토모 장비개방
-悠久に輝く龍頭琴_x000D_
-精霊を宿す髪飾り_x000D_
-まほろばの極衣</t>
+영원히 빛나는 용두금(悠久に輝く龍頭琴)
+졍령이 깃드는 머리장식(精霊を宿す髪飾り)
+마호로바의 극의(まほろばの極衣)</t>
   </si>
   <si>
     <t>伝説の職人の依頼</t>
@@ -603,10 +603,10 @@
   </si>
   <si>
     <t>입수
-カイゼリンシリーズ
+카이제린 시리즈(カイゼリンシリーズ)
 장비개방
-マスターＸシリーズ_x000D_
-桐花・真/三葵・真シリーズ</t>
+마스터Ｘ 시리즈(マスターＸシリーズ)
+동화・진/삼규・진 시리즈(桐花・真/三葵・真シリーズ)</t>
   </si>
   <si>
     <t>ベルナ村の加工屋の依頼1</t>
@@ -619,7 +619,7 @@
   </si>
   <si>
     <t>장비개방
-マスターシリーズ</t>
+마스터 시리즈(マスターシリーズ)</t>
   </si>
   <si>
     <t>ベルナ村の加工屋の依頼2</t>
@@ -632,7 +632,7 @@
   </si>
   <si>
     <t>장비개방
-工房謹製・オオナグリ</t>
+공방근제・오오나구리(工房謹製・オオナグリ)</t>
   </si>
   <si>
     <t>ネコ嬢の依頼1</t>
@@ -645,8 +645,8 @@
   </si>
   <si>
     <t>입수
-ハチミツ x10
-龍歴院ポイント200pts</t>
+벌꿀 x10(ハチミツ x10)
+용역원 포인트 200pts(龍歴院ポイント200pts)</t>
   </si>
   <si>
     <t>ネコ嬢の依頼2</t>
@@ -659,10 +659,10 @@
   </si>
   <si>
     <t>퀘스트 보수
-ふんわり白毛玉
+폭신폭신 하얀 털뭉치(ふんわり白毛玉)
 오토모 장비개방
-プリティネコリボン_x000D_
-プリティネコワンピ</t>
+프리티 고양이 리본(プリティネコリボン)
+프리티 고양이 원피스(プリティネコワンピ)</t>
   </si>
   <si>
     <t>ネコ嬢の依頼3</t>
@@ -675,11 +675,11 @@
   </si>
   <si>
     <t>장비개방
-ムーファＸシリーズ
+무파Ｘ 시리즈(ムーファＸシリーズ)
 오토모 장비개방
-ムーファＸネコウール_x000D_
-ムーファＸネコヘッド_x000D_
-ムーファＸネコスーツ</t>
+무파Ｘ 고양이 울(ムーファＸネコウール)
+무파Ｘ 고양이 헤드(ムーファＸネコヘッド)
+무파Ｘ 고양이 슈트(ムーファＸネコスーツ)</t>
   </si>
   <si>
     <t>酒場の看板娘の依頼(1)</t>
@@ -692,12 +692,12 @@
   </si>
   <si>
     <t>퀘스트 보수
-ふんわり黒毛玉
+폭신폭신 검은 털뭉치(ふんわり黒毛玉)
 오토모 장비개방
-キュートネコリボン_x000D_
-キュートネコワンピ
+큐트 고양이 리본(キュートネコリボン)
+큐트 고양이 원피스(キュートネコワンピ)
 푸기의 옷
-フェニーの服：麗しのフロイライン</t>
+페니의 옷 : 아름다운 프로일라인(フェニーの服：麗しのフロイライン)</t>
   </si>
   <si>
     <t>酒場の看板娘の依頼(2)</t>
@@ -710,7 +710,7 @@
   </si>
   <si>
     <t>입수
-防具合成材・頭 x2</t>
+방어구 합성 소재・머리 x2(防具合成材・頭 x2)</t>
   </si>
   <si>
     <t>ニャント様の依頼</t>
@@ -723,9 +723,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-サンマージ結晶
+섬머지 결정(サンマージ結晶)
 장비개방
-ルーツォ＝スーロ</t>
+루츠오 = 스로(ルーツォ＝スーロ)</t>
   </si>
   <si>
     <t>코코트 마을(ココット村)</t>
@@ -1168,6 +1168,9 @@
   </si>
   <si>
     <t>마을★8 열대에 나타나다, 우라간킨!(熱地に現る、ウラガンキン！)</t>
+  </si>
+  <si>
+    <t>ルームサービス変更可能</t>
   </si>
   <si>
     <t>キャラバンの竜人商人の依頼1</t>
@@ -3260,8 +3263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4579,7 +4582,7 @@
         <v>309</v>
       </c>
       <c r="E77" t="s">
-        <v>109</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
@@ -4587,16 +4590,16 @@
         <v>186</v>
       </c>
       <c r="B78" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C78" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D78" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30">
@@ -4604,16 +4607,16 @@
         <v>186</v>
       </c>
       <c r="B79" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C79" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D79" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30">
@@ -4621,16 +4624,16 @@
         <v>186</v>
       </c>
       <c r="B80" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C80" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D80" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="75">
@@ -4638,16 +4641,16 @@
         <v>186</v>
       </c>
       <c r="B81" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C81" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D81" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="60">
@@ -4655,16 +4658,16 @@
         <v>186</v>
       </c>
       <c r="B82" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C82" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D82" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30">
@@ -4672,16 +4675,16 @@
         <v>186</v>
       </c>
       <c r="B83" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C83" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D83" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="60">
@@ -4689,16 +4692,16 @@
         <v>186</v>
       </c>
       <c r="B84" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C84" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30">
@@ -4706,16 +4709,16 @@
         <v>186</v>
       </c>
       <c r="B85" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C85" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D85" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="30">
@@ -4723,16 +4726,16 @@
         <v>186</v>
       </c>
       <c r="B86" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C86" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D86" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="120">
@@ -4740,16 +4743,16 @@
         <v>186</v>
       </c>
       <c r="B87" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C87" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D87" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30">
@@ -4757,1835 +4760,1835 @@
         <v>186</v>
       </c>
       <c r="B88" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C88" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D88" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30">
       <c r="A89" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B89" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C89" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D89" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="75">
       <c r="A90" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B90" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C90" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D90" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B91" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C91" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D91" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="30">
       <c r="A92" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B92" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C92" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D92" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="75">
       <c r="A93" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B93" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C93" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D93" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30">
       <c r="A94" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B94" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C94" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D94" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="75">
       <c r="A95" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B95" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C95" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D95" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B96" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C96" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B97" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C97" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D97" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="105">
       <c r="A98" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B98" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C98" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D98" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30">
       <c r="A99" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B99" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C99" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D99" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30">
       <c r="A100" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B100" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C100" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D100" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30">
       <c r="A101" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B101" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C101" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D101" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="60">
       <c r="A102" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B102" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C102" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D102" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="60">
       <c r="A103" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B103" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C103" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D103" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="90">
       <c r="A104" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B104" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C104" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D104" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30">
       <c r="A105" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B105" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C105" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D105" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="60">
       <c r="A106" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B106" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C106" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D106" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30">
       <c r="A107" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B107" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C107" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D107" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B108" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C108" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D108" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E108" t="s">
-        <v>109</v>
+        <v>310</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="60">
       <c r="A109" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B109" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C109" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="D109" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30">
       <c r="A110" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B110" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C110" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D110" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="30">
       <c r="A111" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B111" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C111" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="D111" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="90">
       <c r="A112" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B112" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C112" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B113" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C113" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D113" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E113" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30">
       <c r="A114" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B114" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C114" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D114" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="45">
       <c r="A115" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B115" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C115" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="D115" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="105">
       <c r="A116" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B116" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C116" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D116" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="60">
       <c r="A117" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B117" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C117" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="D117" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="105">
       <c r="A118" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B118" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C118" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="D118" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="90">
       <c r="A119" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B119" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C119" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D119" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30">
       <c r="A120" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B120" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C120" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D120" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30">
       <c r="A121" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B121" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C121" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D121" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="45">
       <c r="A122" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B122" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C122" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D122" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="390">
       <c r="A123" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B123" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C123" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D123" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="30">
       <c r="A124" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B124" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C124" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D124" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="90">
       <c r="A125" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B125" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C125" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D125" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="30">
       <c r="A126" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B126" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C126" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D126" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30">
       <c r="A127" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B127" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C127" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D127" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="60">
       <c r="A128" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B128" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C128" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="D128" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30">
       <c r="A129" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B129" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C129" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="D129" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="90">
       <c r="A130" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B130" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C130" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D130" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="90">
       <c r="A131" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B131" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C131" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D131" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="75">
       <c r="A132" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B132" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="C132" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D132" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="75">
       <c r="A133" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B133" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C133" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D133" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="30">
       <c r="A134" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B134" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C134" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D134" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45">
       <c r="A135" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B135" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C135" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45">
       <c r="A136" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B136" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C136" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D136" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="45">
       <c r="A137" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B137" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C137" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D137" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45">
       <c r="A138" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B138" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C138" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D138" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="60">
       <c r="A139" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B139" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C139" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="D139" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="60">
       <c r="A140" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B140" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C140" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D140" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="60">
       <c r="A141" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B141" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C141" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D141" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30">
       <c r="A142" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B142" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C142" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="D142" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30">
       <c r="A143" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B143" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C143" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="D143" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30">
       <c r="A144" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B144" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C144" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="D144" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30">
       <c r="A145" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B145" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C145" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="D145" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="30">
       <c r="A146" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B146" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C146" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D146" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30">
       <c r="A147" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B147" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C147" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="30">
       <c r="A148" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B148" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C148" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D148" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="30">
       <c r="A149" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B149" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C149" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D149" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30">
       <c r="A150" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B150" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C150" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D150" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="90">
       <c r="A151" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B151" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C151" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D151" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="45">
       <c r="A152" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B152" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C152" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="30">
       <c r="A153" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B153" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C153" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D153" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B154" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C154" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D154" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E154" t="s">
-        <v>109</v>
+        <v>310</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="75">
       <c r="A155" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B155" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C155" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="D155" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="75">
       <c r="A156" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B156" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C156" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D156" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="75">
       <c r="A157" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B157" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C157" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D157" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B158" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C158" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D158" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E158" t="s">
-        <v>109</v>
+        <v>310</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="60">
       <c r="A159" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B159" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C159" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="30">
       <c r="A160" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B160" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C160" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="30">
       <c r="A161" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B161" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C161" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D161" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="30">
       <c r="A162" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B162" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C162" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D162" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B163" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C163" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D163" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E163" t="s">
-        <v>109</v>
+        <v>310</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="30">
       <c r="A164" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B164" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C164" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D164" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="60">
       <c r="A165" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B165" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C165" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D165" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="60">
       <c r="A166" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B166" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C166" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="30">
       <c r="A167" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B167" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C167" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D167" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="30">
       <c r="A168" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B168" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C168" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D168" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="30">
       <c r="A169" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B169" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C169" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D169" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="60">
       <c r="A170" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B170" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C170" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="60">
       <c r="A171" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B171" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C171" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D171" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="30">
       <c r="A172" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B172" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C172" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="D172" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="60">
       <c r="A173" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B173" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C173" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D173" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="30">
       <c r="A174" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B174" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C174" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D174" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="60">
       <c r="A175" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B175" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C175" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="D175" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="30">
       <c r="A176" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B176" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C176" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D176" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="30">
       <c r="A177" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B177" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C177" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="D177" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="75">
       <c r="A178" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B178" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C178" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D178" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="60">
       <c r="A179" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B179" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C179" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D179" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="60">
       <c r="A180" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B180" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C180" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D180" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="30">
       <c r="A181" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B181" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="C181" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D181" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="60">
       <c r="A182" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B182" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="C182" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="D182" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="60">
       <c r="A183" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B183" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C183" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D183" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="60">
       <c r="A184" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B184" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="C184" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="D184" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="30">
       <c r="A185" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B185" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C185" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D185" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="30">
       <c r="A186" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B186" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C186" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="D186" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="30">
       <c r="A187" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B187" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C187" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D187" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="30">
       <c r="A188" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B188" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C188" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D188" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="30">
       <c r="A189" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B189" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C189" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D189" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="30">
       <c r="A190" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B190" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C190" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="D190" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="30">
       <c r="A191" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B191" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C191" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D191" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="30">
       <c r="A192" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B192" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C192" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D192" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="30">
       <c r="A193" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B193" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C193" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D193" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="45">
       <c r="A194" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B194" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C194" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D194" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="90">
       <c r="A195" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B195" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C195" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="D195" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
requestQuest: Name translation of equipment and foodstuffs to be opened.(~ココット Town)
</commit_message>
<xml_diff>
--- a/request.xlsx
+++ b/request.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="179016"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="778">
   <si>
     <t>town</t>
   </si>
@@ -589,7 +589,7 @@
 가디언Ｚ 시리즈(ガーディアンＺシリーズ)
 오토모 장비개방
 영원히 빛나는 용두금(悠久に輝く龍頭琴)
-졍령이 깃드는 머리장식(精霊を宿す髪飾り)
+졍령이 깃든 머리장식(精霊を宿す髪飾り)
 마호로바의 극의(まほろばの極衣)</t>
   </si>
   <si>
@@ -740,8 +740,8 @@
     <t>마을★2 란포스들을 토벌해라!(ランポスたちを討伐せよ！)</t>
   </si>
   <si>
-    <t>입수_x000D_
-ココット村の村貢献度100pts</t>
+    <t>입수
+코코트 마을의 마을 공헌도 100pts(ココット村の村貢献度100pts)</t>
   </si>
   <si>
     <t>ココット村の村長の依頼2</t>
@@ -754,11 +754,11 @@
   </si>
   <si>
     <t>장비개방
-ハントシリーズ
+헌트 시리즈(ハントシリーズ)
 오토모 장비개방
-ハントネコナイフ_x000D_
-ハントネコヘルム_x000D_
-ハントネコメイル</t>
+헌트 고양이 나이프(ハントネコナイフ)
+헌트 고양이 헬름(ハントネコヘルム)
+헌트 고양이 메일(ハントネコメイル)</t>
   </si>
   <si>
     <t>ココット村の村長の依頼3</t>
@@ -770,10 +770,6 @@
     <t>마을★3 대괴조 얀쿡을 쓰러뜨려라!(大怪鳥イャンクックを倒せ！)</t>
   </si>
   <si>
-    <t>입수_x000D_
- 龍歴院ポイント500pts</t>
-  </si>
-  <si>
     <t>ココット村の村長の依頼4</t>
   </si>
   <si>
@@ -784,7 +780,7 @@
   </si>
   <si>
     <t>입수
-ココットチケット x2</t>
+코코트 티켓 x2(ココットチケット x2)</t>
   </si>
   <si>
     <t>ココット村の村長の依頼5</t>
@@ -797,10 +793,10 @@
   </si>
   <si>
     <t>입수
-ココットチケット x5_x000D_
-ココット村のヒーローブレイド
+코코트 티켓 x5(ココットチケット x5)
+코코트 마을의 히어로 블레이드(ココット村のヒーローブレイド)
 수기개방
-バレットゲイザーLV2</t>
+블릿 게이저LV2(バレットゲイザーLV2)</t>
   </si>
   <si>
     <t>ココット村の村長の依頼6</t>
@@ -813,7 +809,7 @@
   </si>
   <si>
     <t>입수
-煌竜剣</t>
+황룡검(煌竜剣)</t>
   </si>
   <si>
     <t>ココット村の村長の依頼7</t>
@@ -825,12 +821,12 @@
     <t>마을★10 고난도 : 숲과언덕에서 화룡은 선회한다(高難度：森丘にて火竜は旋廻す)</t>
   </si>
   <si>
-    <t>입수_x000D_
-ココットチケットG_x000D_
-오토모 장비개방_x000D_
-ハントＸネコナイフ_x000D_
-ハントＸネコヘルム_x000D_
-ハントＸネコメイル</t>
+    <t>입수
+코코트 티켓G(ココットチケットG)
+오토모 장비개방
+헌트Ｘ 고양이 나이프(ハントＸネコナイフ)
+헌트Ｘ 고양이 헬름(ハントＸネコヘルム)
+헌트Ｘ 고양이 메일(ハントＸネコメイル)</t>
   </si>
   <si>
     <t>ココット村の受付嬢の依頼1</t>
@@ -846,12 +842,12 @@
   </si>
   <si>
     <t>장비개방
-ほろ酔いビーア_x000D_
-メイド/プライベートシリーズ
+호로요이 피어(ほろ酔いビーア)
+메이드/프라이빗 시리즈(メイド/プライベートシリーズ)
 오토모 장비개방
-ココットネコビーア_x000D_
-メイドネコフード_x000D_
-メイドネコメイル</t>
+코코트 고양이 피어(ココットネコビーア)
+메이드 고양이 후드(メイドネコフード)
+메이드 고양이 메일(メイドネコメイル)</t>
   </si>
   <si>
     <t>ココット村の受付嬢の依頼2</t>
@@ -867,11 +863,11 @@
   </si>
   <si>
     <t>장비개방
-メイドＸ/プライベートＸシリーズ
+메이드Ｘ/프라이빗Ｘ 시리즈(メイドＸ/プライベートＸシリーズ)
 오토모 장비개방
-ココットＸネコビーア_x000D_
-メイドＸネコフード_x000D_
-メイドＸネコメイル</t>
+코코트Ｘ 고양이 피어(ココットＸネコビーア)
+메이드Ｘ 고양이 후드(メイドＸネコフード)
+메이드Ｘ 고양이 메일(メイドＸネコメイル)</t>
   </si>
   <si>
     <t>ミナガルデの看板娘の依頼1</t>
@@ -884,10 +880,10 @@
   </si>
   <si>
     <t>장비개방
-メイドS/プライベートSシリーズ
+메이드Ｓ/프라이빗Ｓ 시리즈(メイドＳ/プライベートＳシリーズ)
 오토모 장비개방
-メイドＳネコフード_x000D_
-メイドＳネコメイル</t>
+메이드Ｓ 고양이 후드(メイドＳネコフード)
+메이드Ｓ 고양이 메일(メイドＳネコメイル)</t>
   </si>
   <si>
     <t>ミナガルデの看板娘の依頼2</t>
@@ -899,8 +895,8 @@
     <t>마을★9 새치기수주 : 알납품(割り込み受注：卵納品)</t>
   </si>
   <si>
-    <t>입수_x000D_
-ココット村の村貢献度300pts</t>
+    <t>입수
+코코트 마을의 마을 공헌도 300pts(ココット村の村貢献度300pts)</t>
   </si>
   <si>
     <t>ミナガルデの看板娘の依頼3</t>
@@ -913,7 +909,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX桃毛獣チケット</t>
+EX도모수 티켓(EX桃毛獣チケット)</t>
   </si>
   <si>
     <t>休息中のハンターの依頼</t>
@@ -926,8 +922,8 @@
   </si>
   <si>
     <t>수기개방
-チャージショットLV2
-身躱し射法LV2</t>
+차지 샷LV2(チャージショットLV2)
+회피사법LV2(身躱し射法LV2)</t>
   </si>
   <si>
     <t>トレジィの依頼1</t>
@@ -940,7 +936,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-オオシッポガエル</t>
+큰 꼬리 개구리(オオシッポガエル)</t>
   </si>
   <si>
     <t>トレジィの依頼2</t>
@@ -953,7 +949,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-ハナスズムシ</t>
+꽃방울벌레(ハナスズムシ)</t>
   </si>
   <si>
     <t>トレジィの依頼3</t>
@@ -966,9 +962,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-キングミート
+킹 미트(キングミート)
 장비개방
-グレイトフルハム</t>
+그레이트풀  햄(グレイトフルハム)</t>
   </si>
   <si>
     <t>トレジィの依頼4</t>
@@ -981,7 +977,7 @@
   </si>
   <si>
     <t>식재
-チョモラン米</t>
+초몰룽쌀(チョモラン米)</t>
   </si>
   <si>
     <t>ヘルブラザーズ・赤鬼の依頼(1)</t>
@@ -994,7 +990,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX火竜チケット</t>
+EX화룡 티켓S(EX火竜チケットS)</t>
   </si>
   <si>
     <t>ヘルブラザーズ・赤鬼の依頼(2)</t>
@@ -1006,226 +1002,219 @@
     <t>집회소★7 하늘의 비룡과 육지의 비룡(空の飛竜と陸の飛竜)</t>
   </si>
   <si>
+    <t>ヘルブラザーズ・赤鬼の依頼2</t>
+  </si>
+  <si>
+    <t>헬 브라더스・적귀의 의뢰2</t>
+  </si>
+  <si>
+    <t>마을★9 굉룡 수렵을 시켜주지!(轟竜の狩猟をさせてやるぜ！)</t>
+  </si>
+  <si>
+    <t>장비개방
+크리스탈 록(クリスタルロック)
+알바레드(アルバレッド)</t>
+  </si>
+  <si>
+    <t>ヘルブラザーズ・赤鬼の依頼3</t>
+  </si>
+  <si>
+    <t>헬 브라더스・적귀의 의뢰3</t>
+  </si>
+  <si>
+    <t>G★2 겸해의 수렵을 시켜주지!(鎌蟹の狩猟をさせてやるぜ！)</t>
+  </si>
+  <si>
+    <t>수기개방
+문 브레이크LV2(ムーンブレイクLV2)
+각충강화LV2(覚蟲強化LV2)</t>
+  </si>
+  <si>
+    <t>ドンドルマの守護兵の依頼1</t>
+  </si>
+  <si>
+    <t>돈도르마 수호병의 의뢰1</t>
+  </si>
+  <si>
+    <t>마을★6 고난도 : 흑랑조는 내려앉았다(高難度：黒狼鳥は舞い降りた)</t>
+  </si>
+  <si>
+    <t>장비개방
+가디언 시리즈(ガーディアンシリーズ)
+가디언U 시리즈(ガーディアンUシリーズ)
+가디언 랜스(ガーディアンランス)</t>
+  </si>
+  <si>
+    <t>ドンドルマの守護兵の依頼2</t>
+  </si>
+  <si>
+    <t>돈도르마 수호병의 의뢰2</t>
+  </si>
+  <si>
+    <t>마을★6 고난도 : 대하룡방위작전!(高難度：対霞龍防衛作戦！)</t>
+  </si>
+  <si>
+    <t>장비개방
+용두금(龍頭琴)
+오토모 장비개방
+영원의 용두금(悠久の龍頭琴)
+영혼이 깃든 머리장식(魂を宿す髪飾り)
+마호로바의 옷(まほろばの衣)</t>
+  </si>
+  <si>
+    <t>ドンドルマの守護兵の依頼3</t>
+  </si>
+  <si>
+    <t>돈도르마 수호병의 의뢰3</t>
+  </si>
+  <si>
+    <t>G★1 숲과언덕의 성가신 괴조씨(森丘の迷惑な怪鳥さん)</t>
+  </si>
+  <si>
+    <t>식재
+큰 돈도르 콩(大ドンドル豆)</t>
+  </si>
+  <si>
+    <t>シナト村の長老の依頼</t>
+  </si>
+  <si>
+    <t>시나토 마을 장로의 의뢰</t>
+  </si>
+  <si>
+    <t>집회소★4 안주로 쓸 간은 하얀간(肴のキモはホワイトレバー)</t>
+  </si>
+  <si>
+    <t>식재
+시나토 날치(シナトビウオ)</t>
+  </si>
+  <si>
+    <t>キャラバンの料理長の依頼1</t>
+  </si>
+  <si>
+    <t>캐러밴 요리장의 의뢰1</t>
+  </si>
+  <si>
+    <t>집회소★1 새로운 식재헌터의 탄생!?(新たな食材ハンターの誕生！？)</t>
+  </si>
+  <si>
+    <t>식재
+치코 옥수수(チココーン)</t>
+  </si>
+  <si>
+    <t>キャラバンの料理長の依頼2</t>
+  </si>
+  <si>
+    <t>캐러밴 요리장의 의뢰2</t>
+  </si>
+  <si>
+    <t>마을★9 설산, 설옥, 설합전!!(雪山、雪玉、雪合戦！！)</t>
+  </si>
+  <si>
+    <t>식재
+대음양・용살(大吟醸・龍ころし)</t>
+  </si>
+  <si>
+    <t>キャラバンの料理長の依頼3</t>
+  </si>
+  <si>
+    <t>캐러밴 요리장의 의뢰3</t>
+  </si>
+  <si>
+    <t>G★2 치코마을을 위협하는 수룡을 사냥해라!(チコ村を脅かす水竜を狩れ！)</t>
+  </si>
+  <si>
+    <t>식재
+천연 치코 복어(天然チコフグ)</t>
+  </si>
+  <si>
+    <t>キャラバンの娘の依頼1</t>
+  </si>
+  <si>
+    <t>캐러밴 아가씨의 의뢰1</t>
+  </si>
+  <si>
+    <t>나구리 마을(ナグリ村) 촌장과 대화</t>
+  </si>
+  <si>
+    <t>식재
+앗뜨앗뜨염통(アツアツハツ)</t>
+  </si>
+  <si>
+    <t>キャラバンの娘の依頼2</t>
+  </si>
+  <si>
+    <t>캐러밴 아가씨의 의뢰2</t>
+  </si>
+  <si>
+    <t>집회소★6 마음을 불태워라, 연석탄!(心を燃やせ、燃石炭！)</t>
+  </si>
+  <si>
+    <t>식재
+마그마돈(マグマトン)</t>
+  </si>
+  <si>
+    <t>キャラバンの娘の依頼3</t>
+  </si>
+  <si>
+    <t>캐러밴 아가씨의 의뢰3</t>
+  </si>
+  <si>
+    <t>마을★8 열대에 나타나다, 우라간킨!(熱地に現る、ウラガンキン！)</t>
+  </si>
+  <si>
+    <t>キャラバンの竜人商人の依頼1</t>
+  </si>
+  <si>
+    <t>캐러밴 용인상인의 의뢰1</t>
+  </si>
+  <si>
+    <t>마을★5 게료스한 계절(ゲリョスな季節)</t>
+  </si>
+  <si>
     <t>퀘스트 보수
-EX火竜チケットS</t>
-  </si>
-  <si>
-    <t>ヘルブラザーズ・赤鬼の依頼2</t>
-  </si>
-  <si>
-    <t>헬 브라더스・적귀의 의뢰2</t>
-  </si>
-  <si>
-    <t>마을★9 굉룡 수렵을 시켜주지!(轟竜の狩猟をさせてやるぜ！)</t>
+유쿠모 시라타마코(ユクモ白玉粉)</t>
+  </si>
+  <si>
+    <t>キャラバンの竜人商人の依頼2</t>
+  </si>
+  <si>
+    <t>캐러밴 용인상인의 의뢰2</t>
+  </si>
+  <si>
+    <t>집회소★3 화석에 잠든 태고의 기억(化石に眠る太古の記憶)</t>
+  </si>
+  <si>
+    <t>퀘스트 보수
+봉제인형 세트(ぬいぐるみセット)</t>
+  </si>
+  <si>
+    <t>キャラバンの竜人商人の依頼3</t>
+  </si>
+  <si>
+    <t>캐러밴 용인상인의 의뢰3</t>
+  </si>
+  <si>
+    <t>집회소★5 설산의 주인, 도도블랑고(雪山の主、ドドブランゴ)</t>
+  </si>
+  <si>
+    <t>퀘스트 보수
+대칠성(オオナナホシ)</t>
+  </si>
+  <si>
+    <t>キャラバンの竜人商人の依頼4</t>
+  </si>
+  <si>
+    <t>캐러밴 용인상인의 의뢰4</t>
+  </si>
+  <si>
+    <t>마을★10 유군령을 가로막는 공폭룡(遺群嶺を塞ぐ恐暴竜)</t>
   </si>
   <si>
     <t>장비개방
-クリスタルロック_x000D_
-アルバレッド</t>
-  </si>
-  <si>
-    <t>ヘルブラザーズ・赤鬼の依頼3</t>
-  </si>
-  <si>
-    <t>헬 브라더스・적귀의 의뢰3</t>
-  </si>
-  <si>
-    <t>G★2 겸해의 수렵을 시켜주지!(鎌蟹の狩猟をさせてやるぜ！)</t>
-  </si>
-  <si>
-    <t>수기개방
-ムーンブレイクLV2
-覚蟲強化LV2</t>
-  </si>
-  <si>
-    <t>ドンドルマの守護兵の依頼1</t>
-  </si>
-  <si>
-    <t>돈도르마 수호병의 의뢰1</t>
-  </si>
-  <si>
-    <t>마을★6 고난도 : 흑랑조는 내려앉았다(高難度：黒狼鳥は舞い降りた)</t>
-  </si>
-  <si>
-    <t>장비개방
-ガーディアンシリーズ_x000D_
-ガーディアンUシリーズ_x000D_
-ガーディアンランス</t>
-  </si>
-  <si>
-    <t>ドンドルマの守護兵の依頼2</t>
-  </si>
-  <si>
-    <t>돈도르마 수호병의 의뢰2</t>
-  </si>
-  <si>
-    <t>마을★6 고난도 : 대하룡방위작전!(高難度：対霞龍防衛作戦！)</t>
-  </si>
-  <si>
-    <t>장비개방
-龍頭琴
-오토모 장비개방
-悠久の龍頭琴_x000D_
-魂を宿す髪飾り_x000D_
-まほろばの衣</t>
-  </si>
-  <si>
-    <t>ドンドルマの守護兵の依頼3</t>
-  </si>
-  <si>
-    <t>돈도르마 수호병의 의뢰3</t>
-  </si>
-  <si>
-    <t>G★1 숲과언덕의 성가신 괴조씨(森丘の迷惑な怪鳥さん)</t>
-  </si>
-  <si>
-    <t>식재
-大ドンドル豆</t>
-  </si>
-  <si>
-    <t>シナト村の長老の依頼</t>
-  </si>
-  <si>
-    <t>시나토 마을 장로의 의뢰</t>
-  </si>
-  <si>
-    <t>집회소★4 안주로 쓸 간은 하얀간(肴のキモはホワイトレバー)</t>
-  </si>
-  <si>
-    <t>식재_x000D_
-シナトビウオ</t>
-  </si>
-  <si>
-    <t>キャラバンの料理長の依頼1</t>
-  </si>
-  <si>
-    <t>캐러밴 요리장의 의뢰1</t>
-  </si>
-  <si>
-    <t>집회소★1 새로운 식재헌터의 탄생!?(新たな食材ハンターの誕生！？)</t>
-  </si>
-  <si>
-    <t>식재_x000D_
-チココーン</t>
-  </si>
-  <si>
-    <t>キャラバンの料理長の依頼2</t>
-  </si>
-  <si>
-    <t>캐러밴 요리장의 의뢰2</t>
-  </si>
-  <si>
-    <t>마을★9 설산, 설옥, 설합전!!(雪山、雪玉、雪合戦！！)</t>
-  </si>
-  <si>
-    <t>식재_x000D_
-大吟醸・龍ころし</t>
-  </si>
-  <si>
-    <t>キャラバンの料理長の依頼3</t>
-  </si>
-  <si>
-    <t>캐러밴 요리장의 의뢰3</t>
-  </si>
-  <si>
-    <t>G★2 치코마을을 위협하는 수룡을 사냥해라!(チコ村を脅かす水竜を狩れ！)</t>
-  </si>
-  <si>
-    <t>식재_x000D_
-天然チコフグ</t>
-  </si>
-  <si>
-    <t>キャラバンの娘の依頼1</t>
-  </si>
-  <si>
-    <t>캐러밴 아가씨의 의뢰1</t>
-  </si>
-  <si>
-    <t>나구리 마을(ナグリ村) 촌장과 대화</t>
-  </si>
-  <si>
-    <t>식재_x000D_
-アツアツハツ</t>
-  </si>
-  <si>
-    <t>キャラバンの娘の依頼2</t>
-  </si>
-  <si>
-    <t>캐러밴 아가씨의 의뢰2</t>
-  </si>
-  <si>
-    <t>집회소★6 마음을 불태워라, 연석탄!(心を燃やせ、燃石炭！)</t>
-  </si>
-  <si>
-    <t>식재_x000D_
-マグマトン</t>
-  </si>
-  <si>
-    <t>キャラバンの娘の依頼3</t>
-  </si>
-  <si>
-    <t>캐러밴 아가씨의 의뢰3</t>
-  </si>
-  <si>
-    <t>마을★8 열대에 나타나다, 우라간킨!(熱地に現る、ウラガンキン！)</t>
-  </si>
-  <si>
-    <t>ルームサービス変更可能</t>
-  </si>
-  <si>
-    <t>キャラバンの竜人商人の依頼1</t>
-  </si>
-  <si>
-    <t>캐러밴 용인상인의 의뢰1</t>
-  </si>
-  <si>
-    <t>마을★5 게료스한 계절(ゲリョスな季節)</t>
-  </si>
-  <si>
-    <t>퀘스트 보수
-ユクモ白玉粉</t>
-  </si>
-  <si>
-    <t>キャラバンの竜人商人の依頼2</t>
-  </si>
-  <si>
-    <t>캐러밴 용인상인의 의뢰2</t>
-  </si>
-  <si>
-    <t>집회소★3 화석에 잠든 태고의 기억(化石に眠る太古の記憶)</t>
-  </si>
-  <si>
-    <t>퀘스트 보수
-ぬいぐるみセット</t>
-  </si>
-  <si>
-    <t>キャラバンの竜人商人の依頼3</t>
-  </si>
-  <si>
-    <t>캐러밴 용인상인의 의뢰3</t>
-  </si>
-  <si>
-    <t>집회소★5 설산의 주인, 도도블랑고(雪山の主、ドドブランゴ)</t>
-  </si>
-  <si>
-    <t>퀘스트 보수
-オオナナホシ</t>
-  </si>
-  <si>
-    <t>キャラバンの竜人商人の依頼4</t>
-  </si>
-  <si>
-    <t>캐러밴 용인상인의 의뢰4</t>
-  </si>
-  <si>
-    <t>마을★10 유군령을 가로막는 공폭룡(遺群嶺を塞ぐ恐暴竜)</t>
-  </si>
-  <si>
-    <t>장비개방
-エルドラジェズル_x000D_
-エルドラカノーネ_x000D_
-ジャギィフェイク_x000D_
-ジャギィＸフェイク</t>
+엘도라 제즐(エルドラジェズル)
+엘도라 카노네(エルドラカノーネ)
+쟈기 페이크(ジャギィフェイク)
+쟈기Ｘ 페이크(ジャギィＸフェイク)</t>
   </si>
   <si>
     <t>交易船の船長の依頼1</t>
@@ -1238,9 +1227,9 @@
   </si>
   <si>
     <t>입수
-謎の武器の秘伝書 x1
-푸기의 옷_x000D_
-カエルのマーチ</t>
+수수께끼의 무기 비전서 x1(謎の武器の秘伝書 x1)
+푸기의 옷
+개구리의 행진(カエルのマーチ)</t>
   </si>
   <si>
     <t>交易船の船長の依頼2</t>
@@ -1253,7 +1242,7 @@
   </si>
   <si>
     <t>입수
-謎の重弩の秘伝書 x1</t>
+수수께끼의 중노 비전서 x1(謎の重弩の秘伝書 x1)</t>
   </si>
   <si>
     <t>交易船の船長の依頼3</t>
@@ -1269,8 +1258,8 @@
   </si>
   <si>
     <t>장비개방
-ホクシン/カイエンシリーズ_x000D_
-GXホクシン/GXカイエンシリーズ</t>
+호쿠신/카이엔 시리즈(ホクシン/カイエンシリーズ)
+GX호쿠신/GX카이엔 시리즈(GXホクシン/GXカイエンシリーズ)</t>
   </si>
   <si>
     <t>交易船の船長の依頼4</t>
@@ -1283,7 +1272,7 @@
   </si>
   <si>
     <t>입수
-南蛮刀</t>
+남만도(南蛮刀)</t>
   </si>
   <si>
     <t>バルバレの仕切り役の依頼1</t>
@@ -1296,7 +1285,13 @@
   </si>
   <si>
     <t>입수
-ギルドチケット x5</t>
+길드 티켓 x5(ギルドチケット x5)
+장비개방
+닌자 소드(ニンジャソード)
+인・천/인・지 시리즈(忍・天/忍・地シリーズ)
+인・공/인・해 시리즈(忍・空/忍・海シリーズ)
+수기개방
+음격진LV3(音撃震LV3)</t>
   </si>
   <si>
     <t>バルバレの仕切り役の依頼2</t>
@@ -1308,16 +1303,6 @@
     <t>집회소★7 시련의 귀결점(試練の帰結点)</t>
   </si>
   <si>
-    <t>입수
-ギルドチケット x5
-장비개방
-ニンジャソード_x000D_
-忍・天/忍・地シリーズ_x000D_
-忍・空/忍・海シリーズ
-수기개방
-音撃震LV3</t>
-  </si>
-  <si>
     <t>バルバレの仕切り役の依頼3</t>
   </si>
   <si>
@@ -1328,7 +1313,7 @@
   </si>
   <si>
     <t>장비개방
-忍・極天/忍・極地シリーズ</t>
+인・극천/인・극지 시리즈(忍・極天/忍・極地シリーズ)</t>
   </si>
   <si>
     <t>폿케 마을(ポッケ村)</t>
@@ -1625,6 +1610,9 @@
   </si>
   <si>
     <t>G★2 부딪혀라 삶☆아프로 소울(ぶつけろ生き様☆アフロソウル)</t>
+  </si>
+  <si>
+    <t>ルームサービス変更可能</t>
   </si>
   <si>
     <t>さすらいのコックの依頼1</t>
@@ -3263,8 +3251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="D83" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4106,7 +4094,7 @@
         <v>197</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30">
@@ -4114,16 +4102,16 @@
         <v>186</v>
       </c>
       <c r="B50" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" t="s">
         <v>199</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>200</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="75">
@@ -4131,16 +4119,16 @@
         <v>186</v>
       </c>
       <c r="B51" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51" t="s">
         <v>203</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>204</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30">
@@ -4148,16 +4136,16 @@
         <v>186</v>
       </c>
       <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" t="s">
         <v>207</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>208</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="90">
@@ -4165,16 +4153,16 @@
         <v>186</v>
       </c>
       <c r="B53" t="s">
+        <v>210</v>
+      </c>
+      <c r="C53" t="s">
         <v>211</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>212</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="105">
@@ -4182,16 +4170,16 @@
         <v>186</v>
       </c>
       <c r="B54" t="s">
+        <v>214</v>
+      </c>
+      <c r="C54" t="s">
         <v>215</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="90">
@@ -4199,16 +4187,16 @@
         <v>186</v>
       </c>
       <c r="B55" t="s">
+        <v>218</v>
+      </c>
+      <c r="C55" t="s">
         <v>219</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="75">
@@ -4216,16 +4204,16 @@
         <v>186</v>
       </c>
       <c r="B56" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" t="s">
         <v>223</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>224</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30">
@@ -4233,16 +4221,16 @@
         <v>186</v>
       </c>
       <c r="B57" t="s">
+        <v>226</v>
+      </c>
+      <c r="C57" t="s">
         <v>227</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>228</v>
       </c>
-      <c r="D57" t="s">
+      <c r="E57" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30">
@@ -4250,16 +4238,16 @@
         <v>186</v>
       </c>
       <c r="B58" t="s">
+        <v>230</v>
+      </c>
+      <c r="C58" t="s">
         <v>231</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>232</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="45">
@@ -4267,16 +4255,16 @@
         <v>186</v>
       </c>
       <c r="B59" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" t="s">
         <v>235</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>236</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30">
@@ -4284,16 +4272,16 @@
         <v>186</v>
       </c>
       <c r="B60" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" t="s">
         <v>239</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>240</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30">
@@ -4301,16 +4289,16 @@
         <v>186</v>
       </c>
       <c r="B61" t="s">
+        <v>242</v>
+      </c>
+      <c r="C61" t="s">
         <v>243</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>244</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="60">
@@ -4318,16 +4306,16 @@
         <v>186</v>
       </c>
       <c r="B62" t="s">
+        <v>246</v>
+      </c>
+      <c r="C62" t="s">
         <v>247</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>248</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30">
@@ -4335,16 +4323,16 @@
         <v>186</v>
       </c>
       <c r="B63" t="s">
+        <v>250</v>
+      </c>
+      <c r="C63" t="s">
         <v>251</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>252</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
@@ -4352,16 +4340,16 @@
         <v>186</v>
       </c>
       <c r="B64" t="s">
+        <v>254</v>
+      </c>
+      <c r="C64" t="s">
         <v>255</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>256</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30">
@@ -4369,16 +4357,16 @@
         <v>186</v>
       </c>
       <c r="B65" t="s">
+        <v>258</v>
+      </c>
+      <c r="C65" t="s">
         <v>259</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>260</v>
       </c>
-      <c r="D65" t="s">
-        <v>261</v>
-      </c>
       <c r="E65" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="45">
@@ -4386,16 +4374,16 @@
         <v>186</v>
       </c>
       <c r="B66" t="s">
+        <v>261</v>
+      </c>
+      <c r="C66" t="s">
+        <v>262</v>
+      </c>
+      <c r="D66" t="s">
         <v>263</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D66" t="s">
-        <v>265</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="45">
@@ -4403,16 +4391,16 @@
         <v>186</v>
       </c>
       <c r="B67" t="s">
+        <v>265</v>
+      </c>
+      <c r="C67" t="s">
+        <v>266</v>
+      </c>
+      <c r="D67" t="s">
         <v>267</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="D67" t="s">
-        <v>269</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="60">
@@ -4420,16 +4408,16 @@
         <v>186</v>
       </c>
       <c r="B68" t="s">
+        <v>269</v>
+      </c>
+      <c r="C68" t="s">
+        <v>270</v>
+      </c>
+      <c r="D68" t="s">
         <v>271</v>
       </c>
-      <c r="C68" t="s">
+      <c r="E68" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="D68" t="s">
-        <v>273</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="90">
@@ -4437,16 +4425,16 @@
         <v>186</v>
       </c>
       <c r="B69" t="s">
+        <v>273</v>
+      </c>
+      <c r="C69" t="s">
+        <v>274</v>
+      </c>
+      <c r="D69" t="s">
         <v>275</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="D69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30">
@@ -4454,16 +4442,16 @@
         <v>186</v>
       </c>
       <c r="B70" t="s">
+        <v>277</v>
+      </c>
+      <c r="C70" t="s">
+        <v>278</v>
+      </c>
+      <c r="D70" t="s">
         <v>279</v>
       </c>
-      <c r="C70" t="s">
+      <c r="E70" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="D70" t="s">
-        <v>281</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="30">
@@ -4471,16 +4459,16 @@
         <v>186</v>
       </c>
       <c r="B71" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" t="s">
+        <v>282</v>
+      </c>
+      <c r="D71" t="s">
         <v>283</v>
       </c>
-      <c r="C71" t="s">
+      <c r="E71" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="D71" t="s">
-        <v>285</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
@@ -4488,16 +4476,16 @@
         <v>186</v>
       </c>
       <c r="B72" t="s">
+        <v>285</v>
+      </c>
+      <c r="C72" t="s">
+        <v>286</v>
+      </c>
+      <c r="D72" t="s">
         <v>287</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="D72" t="s">
-        <v>289</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="30">
@@ -4505,16 +4493,16 @@
         <v>186</v>
       </c>
       <c r="B73" t="s">
+        <v>289</v>
+      </c>
+      <c r="C73" t="s">
+        <v>290</v>
+      </c>
+      <c r="D73" t="s">
         <v>291</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="D73" t="s">
-        <v>293</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
@@ -4522,16 +4510,16 @@
         <v>186</v>
       </c>
       <c r="B74" t="s">
+        <v>293</v>
+      </c>
+      <c r="C74" t="s">
+        <v>294</v>
+      </c>
+      <c r="D74" t="s">
         <v>295</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="D74" t="s">
-        <v>297</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30">
@@ -4539,16 +4527,16 @@
         <v>186</v>
       </c>
       <c r="B75" t="s">
+        <v>297</v>
+      </c>
+      <c r="C75" t="s">
+        <v>298</v>
+      </c>
+      <c r="D75" t="s">
         <v>299</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="D75" t="s">
-        <v>301</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
@@ -4556,16 +4544,16 @@
         <v>186</v>
       </c>
       <c r="B76" t="s">
+        <v>301</v>
+      </c>
+      <c r="C76" t="s">
+        <v>302</v>
+      </c>
+      <c r="D76" t="s">
         <v>303</v>
       </c>
-      <c r="C76" t="s">
+      <c r="E76" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="D76" t="s">
-        <v>305</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4573,16 +4561,16 @@
         <v>186</v>
       </c>
       <c r="B77" t="s">
+        <v>305</v>
+      </c>
+      <c r="C77" t="s">
+        <v>306</v>
+      </c>
+      <c r="D77" t="s">
         <v>307</v>
       </c>
-      <c r="C77" t="s">
-        <v>308</v>
-      </c>
-      <c r="D77" t="s">
-        <v>309</v>
-      </c>
       <c r="E77" t="s">
-        <v>310</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30">
@@ -4590,16 +4578,16 @@
         <v>186</v>
       </c>
       <c r="B78" t="s">
+        <v>308</v>
+      </c>
+      <c r="C78" t="s">
+        <v>309</v>
+      </c>
+      <c r="D78" t="s">
+        <v>310</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>311</v>
-      </c>
-      <c r="C78" t="s">
-        <v>312</v>
-      </c>
-      <c r="D78" t="s">
-        <v>313</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30">
@@ -4607,16 +4595,16 @@
         <v>186</v>
       </c>
       <c r="B79" t="s">
+        <v>312</v>
+      </c>
+      <c r="C79" t="s">
+        <v>313</v>
+      </c>
+      <c r="D79" t="s">
+        <v>314</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="C79" t="s">
-        <v>316</v>
-      </c>
-      <c r="D79" t="s">
-        <v>317</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="30">
@@ -4624,16 +4612,16 @@
         <v>186</v>
       </c>
       <c r="B80" t="s">
+        <v>316</v>
+      </c>
+      <c r="C80" t="s">
+        <v>317</v>
+      </c>
+      <c r="D80" t="s">
+        <v>318</v>
+      </c>
+      <c r="E80" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="C80" t="s">
-        <v>320</v>
-      </c>
-      <c r="D80" t="s">
-        <v>321</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="75">
@@ -4641,16 +4629,16 @@
         <v>186</v>
       </c>
       <c r="B81" t="s">
+        <v>320</v>
+      </c>
+      <c r="C81" t="s">
+        <v>321</v>
+      </c>
+      <c r="D81" t="s">
+        <v>322</v>
+      </c>
+      <c r="E81" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="C81" t="s">
-        <v>324</v>
-      </c>
-      <c r="D81" t="s">
-        <v>325</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="60">
@@ -4658,16 +4646,16 @@
         <v>186</v>
       </c>
       <c r="B82" t="s">
+        <v>324</v>
+      </c>
+      <c r="C82" t="s">
+        <v>325</v>
+      </c>
+      <c r="D82" t="s">
+        <v>326</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="C82" t="s">
-        <v>328</v>
-      </c>
-      <c r="D82" t="s">
-        <v>329</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30">
@@ -4675,16 +4663,16 @@
         <v>186</v>
       </c>
       <c r="B83" t="s">
+        <v>328</v>
+      </c>
+      <c r="C83" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" t="s">
+        <v>330</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="C83" t="s">
-        <v>332</v>
-      </c>
-      <c r="D83" t="s">
-        <v>333</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="60">
@@ -4692,16 +4680,16 @@
         <v>186</v>
       </c>
       <c r="B84" t="s">
+        <v>332</v>
+      </c>
+      <c r="C84" t="s">
+        <v>333</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="C84" t="s">
-        <v>336</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="30">
@@ -4709,33 +4697,33 @@
         <v>186</v>
       </c>
       <c r="B85" t="s">
+        <v>336</v>
+      </c>
+      <c r="C85" t="s">
+        <v>337</v>
+      </c>
+      <c r="D85" t="s">
+        <v>338</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C85" t="s">
-        <v>340</v>
-      </c>
-      <c r="D85" t="s">
-        <v>341</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="30">
+    </row>
+    <row r="86" spans="1:5" ht="120">
       <c r="A86" t="s">
         <v>186</v>
       </c>
       <c r="B86" t="s">
+        <v>340</v>
+      </c>
+      <c r="C86" t="s">
+        <v>341</v>
+      </c>
+      <c r="D86" t="s">
+        <v>342</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="C86" t="s">
-        <v>344</v>
-      </c>
-      <c r="D86" t="s">
-        <v>345</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="120">
@@ -4743,16 +4731,16 @@
         <v>186</v>
       </c>
       <c r="B87" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C87" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D87" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="30">
@@ -4760,1835 +4748,1835 @@
         <v>186</v>
       </c>
       <c r="B88" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C88" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D88" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30">
       <c r="A89" t="s">
+        <v>351</v>
+      </c>
+      <c r="B89" t="s">
+        <v>352</v>
+      </c>
+      <c r="C89" t="s">
+        <v>353</v>
+      </c>
+      <c r="D89" t="s">
+        <v>354</v>
+      </c>
+      <c r="E89" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="B89" t="s">
-        <v>356</v>
-      </c>
-      <c r="C89" t="s">
-        <v>357</v>
-      </c>
-      <c r="D89" t="s">
-        <v>358</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="75">
       <c r="A90" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B90" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C90" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D90" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="30">
       <c r="A91" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B91" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C91" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D91" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="30">
       <c r="A92" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B92" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C92" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D92" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="75">
       <c r="A93" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B93" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C93" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D93" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30">
       <c r="A94" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B94" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C94" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D94" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="75">
       <c r="A95" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B95" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C95" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D95" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
       <c r="A96" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B96" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C96" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
       <c r="A97" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B97" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C97" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D97" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="105">
       <c r="A98" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B98" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C98" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D98" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30">
       <c r="A99" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B99" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C99" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D99" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30">
       <c r="A100" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B100" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C100" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D100" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30">
       <c r="A101" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B101" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C101" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D101" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="60">
       <c r="A102" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B102" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C102" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D102" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="60">
       <c r="A103" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B103" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="C103" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D103" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="90">
       <c r="A104" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B104" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C104" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D104" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30">
       <c r="A105" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B105" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C105" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D105" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="60">
       <c r="A106" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B106" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C106" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D106" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30">
       <c r="A107" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B107" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C107" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D107" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B108" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C108" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D108" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E108" t="s">
-        <v>310</v>
+        <v>431</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="60">
       <c r="A109" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B109" t="s">
+        <v>432</v>
+      </c>
+      <c r="C109" t="s">
+        <v>433</v>
+      </c>
+      <c r="D109" t="s">
+        <v>434</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="C109" t="s">
-        <v>436</v>
-      </c>
-      <c r="D109" t="s">
-        <v>437</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30">
       <c r="A110" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B110" t="s">
+        <v>436</v>
+      </c>
+      <c r="C110" t="s">
+        <v>437</v>
+      </c>
+      <c r="D110" t="s">
+        <v>438</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="C110" t="s">
-        <v>440</v>
-      </c>
-      <c r="D110" t="s">
-        <v>441</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="30">
       <c r="A111" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B111" t="s">
+        <v>440</v>
+      </c>
+      <c r="C111" t="s">
+        <v>441</v>
+      </c>
+      <c r="D111" t="s">
+        <v>442</v>
+      </c>
+      <c r="E111" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="C111" t="s">
-        <v>444</v>
-      </c>
-      <c r="D111" t="s">
-        <v>445</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="90">
       <c r="A112" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B112" t="s">
+        <v>444</v>
+      </c>
+      <c r="C112" t="s">
+        <v>445</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="C112" t="s">
-        <v>448</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B113" t="s">
+        <v>448</v>
+      </c>
+      <c r="C113" t="s">
+        <v>449</v>
+      </c>
+      <c r="D113" t="s">
+        <v>450</v>
+      </c>
+      <c r="E113" t="s">
         <v>451</v>
-      </c>
-      <c r="C113" t="s">
-        <v>452</v>
-      </c>
-      <c r="D113" t="s">
-        <v>453</v>
-      </c>
-      <c r="E113" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30">
       <c r="A114" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B114" t="s">
+        <v>452</v>
+      </c>
+      <c r="C114" t="s">
+        <v>453</v>
+      </c>
+      <c r="D114" t="s">
+        <v>454</v>
+      </c>
+      <c r="E114" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="C114" t="s">
-        <v>456</v>
-      </c>
-      <c r="D114" t="s">
-        <v>457</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="45">
       <c r="A115" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B115" t="s">
+        <v>456</v>
+      </c>
+      <c r="C115" t="s">
+        <v>457</v>
+      </c>
+      <c r="D115" t="s">
+        <v>458</v>
+      </c>
+      <c r="E115" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="C115" t="s">
-        <v>460</v>
-      </c>
-      <c r="D115" t="s">
-        <v>461</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="105">
       <c r="A116" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B116" t="s">
+        <v>460</v>
+      </c>
+      <c r="C116" t="s">
+        <v>461</v>
+      </c>
+      <c r="D116" t="s">
+        <v>462</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>463</v>
-      </c>
-      <c r="C116" t="s">
-        <v>464</v>
-      </c>
-      <c r="D116" t="s">
-        <v>465</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="60">
       <c r="A117" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B117" t="s">
+        <v>464</v>
+      </c>
+      <c r="C117" t="s">
+        <v>465</v>
+      </c>
+      <c r="D117" t="s">
+        <v>466</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="C117" t="s">
-        <v>468</v>
-      </c>
-      <c r="D117" t="s">
-        <v>469</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="105">
       <c r="A118" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B118" t="s">
+        <v>468</v>
+      </c>
+      <c r="C118" t="s">
+        <v>469</v>
+      </c>
+      <c r="D118" t="s">
+        <v>470</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="C118" t="s">
-        <v>472</v>
-      </c>
-      <c r="D118" t="s">
-        <v>473</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="90">
       <c r="A119" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B119" t="s">
+        <v>472</v>
+      </c>
+      <c r="C119" t="s">
+        <v>473</v>
+      </c>
+      <c r="D119" t="s">
+        <v>474</v>
+      </c>
+      <c r="E119" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="C119" t="s">
-        <v>476</v>
-      </c>
-      <c r="D119" t="s">
-        <v>477</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30">
       <c r="A120" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B120" t="s">
+        <v>476</v>
+      </c>
+      <c r="C120" t="s">
+        <v>477</v>
+      </c>
+      <c r="D120" t="s">
+        <v>478</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="C120" t="s">
-        <v>480</v>
-      </c>
-      <c r="D120" t="s">
-        <v>481</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30">
       <c r="A121" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B121" t="s">
+        <v>480</v>
+      </c>
+      <c r="C121" t="s">
+        <v>481</v>
+      </c>
+      <c r="D121" t="s">
+        <v>482</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="C121" t="s">
-        <v>484</v>
-      </c>
-      <c r="D121" t="s">
-        <v>485</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="45">
       <c r="A122" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B122" t="s">
+        <v>484</v>
+      </c>
+      <c r="C122" t="s">
+        <v>485</v>
+      </c>
+      <c r="D122" t="s">
+        <v>486</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="C122" t="s">
-        <v>488</v>
-      </c>
-      <c r="D122" t="s">
-        <v>489</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="390">
       <c r="A123" t="s">
+        <v>488</v>
+      </c>
+      <c r="B123" t="s">
+        <v>489</v>
+      </c>
+      <c r="C123" t="s">
+        <v>490</v>
+      </c>
+      <c r="D123" t="s">
         <v>491</v>
       </c>
-      <c r="B123" t="s">
+      <c r="E123" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="C123" t="s">
-        <v>493</v>
-      </c>
-      <c r="D123" t="s">
-        <v>494</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="30">
       <c r="A124" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B124" t="s">
+        <v>493</v>
+      </c>
+      <c r="C124" t="s">
+        <v>494</v>
+      </c>
+      <c r="D124" t="s">
+        <v>495</v>
+      </c>
+      <c r="E124" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="C124" t="s">
-        <v>497</v>
-      </c>
-      <c r="D124" t="s">
-        <v>498</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="90">
       <c r="A125" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B125" t="s">
+        <v>497</v>
+      </c>
+      <c r="C125" t="s">
+        <v>498</v>
+      </c>
+      <c r="D125" t="s">
+        <v>499</v>
+      </c>
+      <c r="E125" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="C125" t="s">
-        <v>501</v>
-      </c>
-      <c r="D125" t="s">
-        <v>502</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="30">
       <c r="A126" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B126" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C126" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D126" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30">
       <c r="A127" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B127" t="s">
+        <v>504</v>
+      </c>
+      <c r="C127" t="s">
+        <v>505</v>
+      </c>
+      <c r="D127" t="s">
+        <v>506</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="C127" t="s">
-        <v>508</v>
-      </c>
-      <c r="D127" t="s">
-        <v>509</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="60">
       <c r="A128" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B128" t="s">
+        <v>508</v>
+      </c>
+      <c r="C128" t="s">
+        <v>509</v>
+      </c>
+      <c r="D128" t="s">
+        <v>510</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="C128" t="s">
-        <v>512</v>
-      </c>
-      <c r="D128" t="s">
-        <v>513</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30">
       <c r="A129" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B129" t="s">
+        <v>512</v>
+      </c>
+      <c r="C129" t="s">
+        <v>513</v>
+      </c>
+      <c r="D129" t="s">
+        <v>514</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>515</v>
-      </c>
-      <c r="C129" t="s">
-        <v>516</v>
-      </c>
-      <c r="D129" t="s">
-        <v>517</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="90">
       <c r="A130" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B130" t="s">
+        <v>516</v>
+      </c>
+      <c r="C130" t="s">
+        <v>517</v>
+      </c>
+      <c r="D130" t="s">
+        <v>518</v>
+      </c>
+      <c r="E130" s="1" t="s">
         <v>519</v>
-      </c>
-      <c r="C130" t="s">
-        <v>520</v>
-      </c>
-      <c r="D130" t="s">
-        <v>521</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="90">
       <c r="A131" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B131" t="s">
+        <v>520</v>
+      </c>
+      <c r="C131" t="s">
+        <v>521</v>
+      </c>
+      <c r="D131" t="s">
+        <v>522</v>
+      </c>
+      <c r="E131" s="1" t="s">
         <v>523</v>
-      </c>
-      <c r="C131" t="s">
-        <v>524</v>
-      </c>
-      <c r="D131" t="s">
-        <v>525</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="75">
       <c r="A132" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B132" t="s">
+        <v>524</v>
+      </c>
+      <c r="C132" t="s">
+        <v>525</v>
+      </c>
+      <c r="D132" t="s">
+        <v>526</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="C132" t="s">
-        <v>528</v>
-      </c>
-      <c r="D132" t="s">
-        <v>529</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="75">
       <c r="A133" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B133" t="s">
+        <v>528</v>
+      </c>
+      <c r="C133" t="s">
+        <v>529</v>
+      </c>
+      <c r="D133" t="s">
+        <v>530</v>
+      </c>
+      <c r="E133" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="C133" t="s">
-        <v>532</v>
-      </c>
-      <c r="D133" t="s">
-        <v>533</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="30">
       <c r="A134" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B134" t="s">
+        <v>532</v>
+      </c>
+      <c r="C134" t="s">
+        <v>533</v>
+      </c>
+      <c r="D134" t="s">
+        <v>534</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>535</v>
-      </c>
-      <c r="C134" t="s">
-        <v>536</v>
-      </c>
-      <c r="D134" t="s">
-        <v>537</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45">
       <c r="A135" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B135" t="s">
+        <v>536</v>
+      </c>
+      <c r="C135" t="s">
+        <v>537</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E135" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="C135" t="s">
-        <v>540</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45">
       <c r="A136" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B136" t="s">
+        <v>540</v>
+      </c>
+      <c r="C136" t="s">
+        <v>541</v>
+      </c>
+      <c r="D136" t="s">
+        <v>542</v>
+      </c>
+      <c r="E136" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="C136" t="s">
-        <v>544</v>
-      </c>
-      <c r="D136" t="s">
-        <v>545</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="45">
       <c r="A137" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B137" t="s">
+        <v>544</v>
+      </c>
+      <c r="C137" t="s">
+        <v>545</v>
+      </c>
+      <c r="D137" t="s">
+        <v>546</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="C137" t="s">
-        <v>548</v>
-      </c>
-      <c r="D137" t="s">
-        <v>549</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45">
       <c r="A138" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B138" t="s">
+        <v>548</v>
+      </c>
+      <c r="C138" t="s">
+        <v>549</v>
+      </c>
+      <c r="D138" t="s">
+        <v>550</v>
+      </c>
+      <c r="E138" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="C138" t="s">
-        <v>552</v>
-      </c>
-      <c r="D138" t="s">
-        <v>553</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="60">
       <c r="A139" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B139" t="s">
+        <v>552</v>
+      </c>
+      <c r="C139" t="s">
+        <v>553</v>
+      </c>
+      <c r="D139" t="s">
+        <v>554</v>
+      </c>
+      <c r="E139" s="1" t="s">
         <v>555</v>
-      </c>
-      <c r="C139" t="s">
-        <v>556</v>
-      </c>
-      <c r="D139" t="s">
-        <v>557</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="60">
       <c r="A140" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B140" t="s">
+        <v>556</v>
+      </c>
+      <c r="C140" t="s">
+        <v>557</v>
+      </c>
+      <c r="D140" t="s">
+        <v>558</v>
+      </c>
+      <c r="E140" s="1" t="s">
         <v>559</v>
-      </c>
-      <c r="C140" t="s">
-        <v>560</v>
-      </c>
-      <c r="D140" t="s">
-        <v>561</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="60">
       <c r="A141" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B141" t="s">
+        <v>560</v>
+      </c>
+      <c r="C141" t="s">
+        <v>561</v>
+      </c>
+      <c r="D141" t="s">
+        <v>562</v>
+      </c>
+      <c r="E141" s="1" t="s">
         <v>563</v>
-      </c>
-      <c r="C141" t="s">
-        <v>564</v>
-      </c>
-      <c r="D141" t="s">
-        <v>565</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30">
       <c r="A142" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B142" t="s">
+        <v>564</v>
+      </c>
+      <c r="C142" t="s">
+        <v>565</v>
+      </c>
+      <c r="D142" t="s">
+        <v>566</v>
+      </c>
+      <c r="E142" s="1" t="s">
         <v>567</v>
-      </c>
-      <c r="C142" t="s">
-        <v>568</v>
-      </c>
-      <c r="D142" t="s">
-        <v>569</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30">
       <c r="A143" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B143" t="s">
+        <v>568</v>
+      </c>
+      <c r="C143" t="s">
+        <v>569</v>
+      </c>
+      <c r="D143" t="s">
+        <v>570</v>
+      </c>
+      <c r="E143" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="C143" t="s">
-        <v>572</v>
-      </c>
-      <c r="D143" t="s">
-        <v>573</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30">
       <c r="A144" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B144" t="s">
+        <v>572</v>
+      </c>
+      <c r="C144" t="s">
+        <v>573</v>
+      </c>
+      <c r="D144" t="s">
+        <v>574</v>
+      </c>
+      <c r="E144" s="1" t="s">
         <v>575</v>
-      </c>
-      <c r="C144" t="s">
-        <v>576</v>
-      </c>
-      <c r="D144" t="s">
-        <v>577</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30">
       <c r="A145" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B145" t="s">
+        <v>576</v>
+      </c>
+      <c r="C145" t="s">
+        <v>577</v>
+      </c>
+      <c r="D145" t="s">
+        <v>578</v>
+      </c>
+      <c r="E145" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="C145" t="s">
-        <v>580</v>
-      </c>
-      <c r="D145" t="s">
-        <v>581</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="30">
       <c r="A146" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B146" t="s">
+        <v>580</v>
+      </c>
+      <c r="C146" t="s">
+        <v>581</v>
+      </c>
+      <c r="D146" t="s">
+        <v>582</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="C146" t="s">
-        <v>584</v>
-      </c>
-      <c r="D146" t="s">
-        <v>585</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30">
       <c r="A147" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B147" t="s">
+        <v>584</v>
+      </c>
+      <c r="C147" t="s">
+        <v>585</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="E147" s="1" t="s">
         <v>587</v>
-      </c>
-      <c r="C147" t="s">
-        <v>588</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="30">
       <c r="A148" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B148" t="s">
+        <v>588</v>
+      </c>
+      <c r="C148" t="s">
+        <v>589</v>
+      </c>
+      <c r="D148" t="s">
+        <v>590</v>
+      </c>
+      <c r="E148" s="1" t="s">
         <v>591</v>
-      </c>
-      <c r="C148" t="s">
-        <v>592</v>
-      </c>
-      <c r="D148" t="s">
-        <v>593</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="30">
       <c r="A149" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B149" t="s">
+        <v>592</v>
+      </c>
+      <c r="C149" t="s">
+        <v>593</v>
+      </c>
+      <c r="D149" t="s">
+        <v>594</v>
+      </c>
+      <c r="E149" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="C149" t="s">
-        <v>596</v>
-      </c>
-      <c r="D149" t="s">
-        <v>597</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30">
       <c r="A150" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B150" t="s">
+        <v>596</v>
+      </c>
+      <c r="C150" t="s">
+        <v>597</v>
+      </c>
+      <c r="D150" t="s">
+        <v>598</v>
+      </c>
+      <c r="E150" s="1" t="s">
         <v>599</v>
-      </c>
-      <c r="C150" t="s">
-        <v>600</v>
-      </c>
-      <c r="D150" t="s">
-        <v>601</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="90">
       <c r="A151" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B151" t="s">
+        <v>600</v>
+      </c>
+      <c r="C151" t="s">
+        <v>601</v>
+      </c>
+      <c r="D151" t="s">
+        <v>602</v>
+      </c>
+      <c r="E151" s="1" t="s">
         <v>603</v>
-      </c>
-      <c r="C151" t="s">
-        <v>604</v>
-      </c>
-      <c r="D151" t="s">
-        <v>605</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="45">
       <c r="A152" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B152" t="s">
+        <v>604</v>
+      </c>
+      <c r="C152" t="s">
+        <v>605</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="E152" s="1" t="s">
         <v>607</v>
-      </c>
-      <c r="C152" t="s">
-        <v>608</v>
-      </c>
-      <c r="D152" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="30">
       <c r="A153" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B153" t="s">
+        <v>608</v>
+      </c>
+      <c r="C153" t="s">
+        <v>609</v>
+      </c>
+      <c r="D153" t="s">
+        <v>610</v>
+      </c>
+      <c r="E153" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="C153" t="s">
-        <v>612</v>
-      </c>
-      <c r="D153" t="s">
-        <v>613</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B154" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C154" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D154" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="E154" t="s">
-        <v>310</v>
+        <v>431</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="75">
       <c r="A155" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B155" t="s">
+        <v>615</v>
+      </c>
+      <c r="C155" t="s">
+        <v>616</v>
+      </c>
+      <c r="D155" t="s">
+        <v>617</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>618</v>
-      </c>
-      <c r="C155" t="s">
-        <v>619</v>
-      </c>
-      <c r="D155" t="s">
-        <v>620</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="75">
       <c r="A156" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B156" t="s">
+        <v>619</v>
+      </c>
+      <c r="C156" t="s">
+        <v>620</v>
+      </c>
+      <c r="D156" t="s">
+        <v>621</v>
+      </c>
+      <c r="E156" s="1" t="s">
         <v>622</v>
-      </c>
-      <c r="C156" t="s">
-        <v>623</v>
-      </c>
-      <c r="D156" t="s">
-        <v>624</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="75">
       <c r="A157" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B157" t="s">
+        <v>623</v>
+      </c>
+      <c r="C157" t="s">
+        <v>624</v>
+      </c>
+      <c r="D157" t="s">
+        <v>625</v>
+      </c>
+      <c r="E157" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="C157" t="s">
-        <v>627</v>
-      </c>
-      <c r="D157" t="s">
-        <v>628</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B158" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C158" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D158" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E158" t="s">
-        <v>310</v>
+        <v>431</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="60">
       <c r="A159" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B159" t="s">
+        <v>630</v>
+      </c>
+      <c r="C159" t="s">
+        <v>631</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="E159" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="C159" t="s">
-        <v>634</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="30">
       <c r="A160" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B160" t="s">
+        <v>634</v>
+      </c>
+      <c r="C160" t="s">
+        <v>635</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="E160" s="1" t="s">
         <v>637</v>
-      </c>
-      <c r="C160" t="s">
-        <v>638</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="30">
       <c r="A161" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B161" t="s">
+        <v>638</v>
+      </c>
+      <c r="C161" t="s">
+        <v>639</v>
+      </c>
+      <c r="D161" t="s">
+        <v>640</v>
+      </c>
+      <c r="E161" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="C161" t="s">
-        <v>642</v>
-      </c>
-      <c r="D161" t="s">
-        <v>643</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="30">
       <c r="A162" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B162" t="s">
+        <v>642</v>
+      </c>
+      <c r="C162" t="s">
+        <v>643</v>
+      </c>
+      <c r="D162" t="s">
+        <v>644</v>
+      </c>
+      <c r="E162" s="1" t="s">
         <v>645</v>
-      </c>
-      <c r="C162" t="s">
-        <v>646</v>
-      </c>
-      <c r="D162" t="s">
-        <v>647</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B163" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C163" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D163" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="E163" t="s">
-        <v>310</v>
+        <v>431</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="30">
       <c r="A164" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B164" t="s">
+        <v>649</v>
+      </c>
+      <c r="C164" t="s">
+        <v>650</v>
+      </c>
+      <c r="D164" t="s">
+        <v>651</v>
+      </c>
+      <c r="E164" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="C164" t="s">
-        <v>653</v>
-      </c>
-      <c r="D164" t="s">
-        <v>654</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="60">
       <c r="A165" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B165" t="s">
+        <v>653</v>
+      </c>
+      <c r="C165" t="s">
+        <v>654</v>
+      </c>
+      <c r="D165" t="s">
+        <v>655</v>
+      </c>
+      <c r="E165" s="1" t="s">
         <v>656</v>
-      </c>
-      <c r="C165" t="s">
-        <v>657</v>
-      </c>
-      <c r="D165" t="s">
-        <v>658</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="60">
       <c r="A166" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B166" t="s">
+        <v>657</v>
+      </c>
+      <c r="C166" t="s">
+        <v>658</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E166" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="C166" t="s">
-        <v>661</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="30">
       <c r="A167" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B167" t="s">
+        <v>661</v>
+      </c>
+      <c r="C167" t="s">
+        <v>662</v>
+      </c>
+      <c r="D167" t="s">
+        <v>663</v>
+      </c>
+      <c r="E167" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="C167" t="s">
-        <v>665</v>
-      </c>
-      <c r="D167" t="s">
-        <v>666</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="30">
       <c r="A168" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B168" t="s">
+        <v>665</v>
+      </c>
+      <c r="C168" t="s">
+        <v>666</v>
+      </c>
+      <c r="D168" t="s">
+        <v>667</v>
+      </c>
+      <c r="E168" s="1" t="s">
         <v>668</v>
-      </c>
-      <c r="C168" t="s">
-        <v>669</v>
-      </c>
-      <c r="D168" t="s">
-        <v>670</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="30">
       <c r="A169" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B169" t="s">
+        <v>669</v>
+      </c>
+      <c r="C169" t="s">
+        <v>670</v>
+      </c>
+      <c r="D169" t="s">
+        <v>671</v>
+      </c>
+      <c r="E169" s="1" t="s">
         <v>672</v>
-      </c>
-      <c r="C169" t="s">
-        <v>673</v>
-      </c>
-      <c r="D169" t="s">
-        <v>674</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="60">
       <c r="A170" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B170" t="s">
+        <v>673</v>
+      </c>
+      <c r="C170" t="s">
+        <v>674</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="E170" s="1" t="s">
         <v>676</v>
-      </c>
-      <c r="C170" t="s">
-        <v>677</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="60">
       <c r="A171" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B171" t="s">
+        <v>677</v>
+      </c>
+      <c r="C171" t="s">
+        <v>678</v>
+      </c>
+      <c r="D171" t="s">
+        <v>679</v>
+      </c>
+      <c r="E171" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="C171" t="s">
-        <v>681</v>
-      </c>
-      <c r="D171" t="s">
-        <v>682</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="30">
       <c r="A172" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B172" t="s">
+        <v>681</v>
+      </c>
+      <c r="C172" t="s">
+        <v>682</v>
+      </c>
+      <c r="D172" t="s">
+        <v>683</v>
+      </c>
+      <c r="E172" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="C172" t="s">
-        <v>685</v>
-      </c>
-      <c r="D172" t="s">
-        <v>686</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="60">
       <c r="A173" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B173" t="s">
+        <v>685</v>
+      </c>
+      <c r="C173" t="s">
+        <v>686</v>
+      </c>
+      <c r="D173" t="s">
+        <v>687</v>
+      </c>
+      <c r="E173" s="1" t="s">
         <v>688</v>
-      </c>
-      <c r="C173" t="s">
-        <v>689</v>
-      </c>
-      <c r="D173" t="s">
-        <v>690</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="30">
       <c r="A174" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B174" t="s">
+        <v>689</v>
+      </c>
+      <c r="C174" t="s">
+        <v>690</v>
+      </c>
+      <c r="D174" t="s">
+        <v>691</v>
+      </c>
+      <c r="E174" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="C174" t="s">
-        <v>693</v>
-      </c>
-      <c r="D174" t="s">
-        <v>694</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="60">
       <c r="A175" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B175" t="s">
+        <v>693</v>
+      </c>
+      <c r="C175" t="s">
+        <v>694</v>
+      </c>
+      <c r="D175" t="s">
+        <v>695</v>
+      </c>
+      <c r="E175" s="1" t="s">
         <v>696</v>
-      </c>
-      <c r="C175" t="s">
-        <v>697</v>
-      </c>
-      <c r="D175" t="s">
-        <v>698</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="30">
       <c r="A176" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B176" t="s">
+        <v>697</v>
+      </c>
+      <c r="C176" t="s">
+        <v>698</v>
+      </c>
+      <c r="D176" t="s">
+        <v>699</v>
+      </c>
+      <c r="E176" s="1" t="s">
         <v>700</v>
-      </c>
-      <c r="C176" t="s">
-        <v>701</v>
-      </c>
-      <c r="D176" t="s">
-        <v>702</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="30">
       <c r="A177" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B177" t="s">
+        <v>701</v>
+      </c>
+      <c r="C177" t="s">
+        <v>702</v>
+      </c>
+      <c r="D177" t="s">
+        <v>703</v>
+      </c>
+      <c r="E177" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="C177" t="s">
-        <v>705</v>
-      </c>
-      <c r="D177" t="s">
-        <v>706</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="75">
       <c r="A178" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B178" t="s">
+        <v>705</v>
+      </c>
+      <c r="C178" t="s">
+        <v>706</v>
+      </c>
+      <c r="D178" t="s">
+        <v>707</v>
+      </c>
+      <c r="E178" s="1" t="s">
         <v>708</v>
-      </c>
-      <c r="C178" t="s">
-        <v>709</v>
-      </c>
-      <c r="D178" t="s">
-        <v>710</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="60">
       <c r="A179" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B179" t="s">
+        <v>709</v>
+      </c>
+      <c r="C179" t="s">
+        <v>710</v>
+      </c>
+      <c r="D179" t="s">
+        <v>711</v>
+      </c>
+      <c r="E179" s="1" t="s">
         <v>712</v>
-      </c>
-      <c r="C179" t="s">
-        <v>713</v>
-      </c>
-      <c r="D179" t="s">
-        <v>714</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="60">
       <c r="A180" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B180" t="s">
+        <v>713</v>
+      </c>
+      <c r="C180" t="s">
+        <v>714</v>
+      </c>
+      <c r="D180" t="s">
+        <v>715</v>
+      </c>
+      <c r="E180" s="1" t="s">
         <v>716</v>
-      </c>
-      <c r="C180" t="s">
-        <v>717</v>
-      </c>
-      <c r="D180" t="s">
-        <v>718</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="30">
       <c r="A181" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B181" t="s">
+        <v>717</v>
+      </c>
+      <c r="C181" t="s">
+        <v>718</v>
+      </c>
+      <c r="D181" t="s">
+        <v>719</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>720</v>
-      </c>
-      <c r="C181" t="s">
-        <v>721</v>
-      </c>
-      <c r="D181" t="s">
-        <v>722</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="60">
       <c r="A182" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B182" t="s">
+        <v>721</v>
+      </c>
+      <c r="C182" t="s">
+        <v>722</v>
+      </c>
+      <c r="D182" t="s">
+        <v>723</v>
+      </c>
+      <c r="E182" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="C182" t="s">
-        <v>725</v>
-      </c>
-      <c r="D182" t="s">
-        <v>726</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="60">
       <c r="A183" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B183" t="s">
+        <v>725</v>
+      </c>
+      <c r="C183" t="s">
+        <v>726</v>
+      </c>
+      <c r="D183" t="s">
+        <v>727</v>
+      </c>
+      <c r="E183" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="C183" t="s">
-        <v>729</v>
-      </c>
-      <c r="D183" t="s">
-        <v>730</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="60">
       <c r="A184" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B184" t="s">
+        <v>729</v>
+      </c>
+      <c r="C184" t="s">
+        <v>730</v>
+      </c>
+      <c r="D184" t="s">
+        <v>731</v>
+      </c>
+      <c r="E184" s="1" t="s">
         <v>732</v>
-      </c>
-      <c r="C184" t="s">
-        <v>733</v>
-      </c>
-      <c r="D184" t="s">
-        <v>734</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>735</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="30">
       <c r="A185" t="s">
+        <v>733</v>
+      </c>
+      <c r="B185" t="s">
+        <v>734</v>
+      </c>
+      <c r="C185" t="s">
+        <v>735</v>
+      </c>
+      <c r="D185" t="s">
         <v>736</v>
       </c>
-      <c r="B185" t="s">
+      <c r="E185" s="1" t="s">
         <v>737</v>
-      </c>
-      <c r="C185" t="s">
-        <v>738</v>
-      </c>
-      <c r="D185" t="s">
-        <v>739</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="30">
       <c r="A186" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B186" t="s">
+        <v>738</v>
+      </c>
+      <c r="C186" t="s">
+        <v>739</v>
+      </c>
+      <c r="D186" t="s">
+        <v>740</v>
+      </c>
+      <c r="E186" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="C186" t="s">
-        <v>742</v>
-      </c>
-      <c r="D186" t="s">
-        <v>743</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>744</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="30">
       <c r="A187" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B187" t="s">
+        <v>742</v>
+      </c>
+      <c r="C187" t="s">
+        <v>743</v>
+      </c>
+      <c r="D187" t="s">
+        <v>744</v>
+      </c>
+      <c r="E187" s="1" t="s">
         <v>745</v>
-      </c>
-      <c r="C187" t="s">
-        <v>746</v>
-      </c>
-      <c r="D187" t="s">
-        <v>747</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="30">
       <c r="A188" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B188" t="s">
+        <v>746</v>
+      </c>
+      <c r="C188" t="s">
+        <v>747</v>
+      </c>
+      <c r="D188" t="s">
+        <v>748</v>
+      </c>
+      <c r="E188" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="C188" t="s">
-        <v>750</v>
-      </c>
-      <c r="D188" t="s">
-        <v>751</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="30">
       <c r="A189" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B189" t="s">
+        <v>750</v>
+      </c>
+      <c r="C189" t="s">
+        <v>751</v>
+      </c>
+      <c r="D189" t="s">
+        <v>752</v>
+      </c>
+      <c r="E189" s="1" t="s">
         <v>753</v>
-      </c>
-      <c r="C189" t="s">
-        <v>754</v>
-      </c>
-      <c r="D189" t="s">
-        <v>755</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>756</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="30">
       <c r="A190" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B190" t="s">
+        <v>754</v>
+      </c>
+      <c r="C190" t="s">
+        <v>755</v>
+      </c>
+      <c r="D190" t="s">
+        <v>756</v>
+      </c>
+      <c r="E190" s="1" t="s">
         <v>757</v>
-      </c>
-      <c r="C190" t="s">
-        <v>758</v>
-      </c>
-      <c r="D190" t="s">
-        <v>759</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="30">
       <c r="A191" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B191" t="s">
+        <v>758</v>
+      </c>
+      <c r="C191" t="s">
+        <v>759</v>
+      </c>
+      <c r="D191" t="s">
+        <v>760</v>
+      </c>
+      <c r="E191" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="C191" t="s">
-        <v>762</v>
-      </c>
-      <c r="D191" t="s">
-        <v>763</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="30">
       <c r="A192" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B192" t="s">
+        <v>762</v>
+      </c>
+      <c r="C192" t="s">
+        <v>763</v>
+      </c>
+      <c r="D192" t="s">
+        <v>764</v>
+      </c>
+      <c r="E192" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="C192" t="s">
-        <v>766</v>
-      </c>
-      <c r="D192" t="s">
-        <v>767</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="30">
       <c r="A193" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B193" t="s">
+        <v>766</v>
+      </c>
+      <c r="C193" t="s">
+        <v>767</v>
+      </c>
+      <c r="D193" t="s">
+        <v>768</v>
+      </c>
+      <c r="E193" s="1" t="s">
         <v>769</v>
-      </c>
-      <c r="C193" t="s">
-        <v>770</v>
-      </c>
-      <c r="D193" t="s">
-        <v>771</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="45">
       <c r="A194" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B194" t="s">
+        <v>770</v>
+      </c>
+      <c r="C194" t="s">
+        <v>771</v>
+      </c>
+      <c r="D194" t="s">
+        <v>772</v>
+      </c>
+      <c r="E194" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="C194" t="s">
-        <v>774</v>
-      </c>
-      <c r="D194" t="s">
-        <v>775</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="90">
       <c r="A195" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="B195" t="s">
+        <v>774</v>
+      </c>
+      <c r="C195" t="s">
+        <v>775</v>
+      </c>
+      <c r="D195" t="s">
+        <v>776</v>
+      </c>
+      <c r="E195" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="C195" t="s">
-        <v>778</v>
-      </c>
-      <c r="D195" t="s">
-        <v>779</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
requestQuest: Name translation of equipment and foodstuffs to be opened.(~ポッケ Town)
</commit_message>
<xml_diff>
--- a/request.xlsx
+++ b/request.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1328,8 +1328,8 @@
     <t>마을★2 기아노스들을 토벌해라!(ギアノスたちを討伐せよ！)</t>
   </si>
   <si>
-    <t>입수_x000D_
-ポッケ村の村貢献度100pts</t>
+    <t>입수
+폿케 마을의 마을 공헌도 100pts(ポッケ村の村貢献度100pts)</t>
   </si>
   <si>
     <t>ポッケ村の村長の依頼2</t>
@@ -1342,10 +1342,10 @@
   </si>
   <si>
     <t>장비개방
-マフモフシリーズ
+마후모후 시리즈(マフモフシリーズ)
 오토모 장비개방
-マフモフネコフード_x000D_
-マフモフネコベスト</t>
+마후모후 고양이 후드(マフモフネコフード)
+마후모후 고양이 베스트(マフモフネコベスト)</t>
   </si>
   <si>
     <t>ポッケ村の村長の依頼3</t>
@@ -1357,10 +1357,6 @@
     <t>마을★3 설산에 숨어있는 그림자(雪山に潜む影)</t>
   </si>
   <si>
-    <t>입수_x000D_
-龍歴院ポイント500pts</t>
-  </si>
-  <si>
     <t>ポッケ村の村長の依頼4</t>
   </si>
   <si>
@@ -1371,7 +1367,7 @@
   </si>
   <si>
     <t>입수
-ポッケチケット x2</t>
+폿케 티켓 x2(ポッケチケット x2)</t>
   </si>
   <si>
     <t>ポッケ村の村長の依頼5</t>
@@ -1384,10 +1380,10 @@
   </si>
   <si>
     <t>입수
-ポッケチケット x5_x000D_
-洞窟の巨大剣が採掘可能
-수기개방_x000D_
-タイフーントリガーLV2</t>
+폿케 티켓 x5(ポッケチケット x5)
+동굴의 거대검 채굴가능(洞窟の巨大剣が採掘可能)
+수기개방
+타이푼 트리거 LV2(タイフーントリガーLV2)</t>
   </si>
   <si>
     <t>ポッケ村の村長の依頼6</t>
@@ -1400,7 +1396,7 @@
   </si>
   <si>
     <t>입수
-鷹見の羽飾り</t>
+응견의 깃털 장식(鷹見の羽飾り)</t>
   </si>
   <si>
     <t>ポッケ村の村長の依頼7</t>
@@ -1413,10 +1409,10 @@
   </si>
   <si>
     <t>입수
-ポッケチケットG
+폿케 티켓G(ポッケチケットG)
 오토모 장비개방
-マフモフＸネコフード_x000D_
-マフモフＸネコベスト</t>
+마후모후Ｘ 고양이 후드(マフモフＸネコフード)
+마후모후Ｘ 고양이 베스트(マフモフＸネコベスト)</t>
   </si>
   <si>
     <t>ポッケ村の受付嬢の依頼1</t>
@@ -1432,12 +1428,12 @@
   </si>
   <si>
     <t>장비개방
-掃棍ミガキ_x000D_
-ヘルパー/ヒーラーシリーズ
+소곤닦기(掃棍ミガキ)
+헬퍼/힐러 시리즈(ヘルパー/ヒーラーシリーズ)
 오토모 장비개방
-ポッケネコモップ_x000D_
-ヘルパーネコフード_x000D_
-ヘルパーネコメイル</t>
+폿케 고양이 대걸레(ポッケネコモップ)
+헬퍼 고양이 후드(ヘルパーネコフード)
+헬퍼 고양이 메일(ヘルパーネコメイル)</t>
   </si>
   <si>
     <t>ポッケ村の受付嬢の依頼2</t>
@@ -1450,12 +1446,12 @@
   </si>
   <si>
     <t>장비개방
-ヘルパーＸ/ヒーラーＸシリーズ_x000D_
-ヘルパーＺ/ヒーラーＺシリーズ
+헬퍼Ｘ/힐러Ｘ 시리즈(ヘルパーＸ/ヒーラーＸシリーズ)
+헬퍼Ｚ/힐러Ｚ 시리즈(ヘルパーＺ/ヒーラーＺシリーズ)
 오토모 장비개방
-ポッケＸネコモップ_x000D_
-ヘルパーＸネコフード_x000D_
-ヘルパーＸネコメイル</t>
+폿케Ｘ 고양이 대걸레(ポッケＸネコモップ)
+헬퍼Ｘ 고양이 후드(ヘルパーＸネコフード)
+헬퍼Ｘ 고양이 메일(ヘルパーＸネコメイル)</t>
   </si>
   <si>
     <t>ジャンボ村の看板娘の依頼</t>
@@ -1468,12 +1464,12 @@
   </si>
   <si>
     <t>장비개방
-ヘルパーS/ヒーラーSシリーズ_x000D_
-ヘルパーU/ヒーラーUシリーズ
+헬퍼Ｓ/힐러Ｓ 시리즈(ヘルパーＳ/ヒーラーＳシリーズ)
+헬퍼U/힐러U 시리즈(ヘルパーU/ヒーラーUシリーズ)
 오토모 장비개방
-ポッケＳネコモップ_x000D_
-ヘルパーＳネコフード_x000D_
-ヘルパーＳネコメイル</t>
+폿케Ｓ 고양이 대걸레(ポッケＳネコモップ)
+헬퍼Ｓ 고양이 후드(ヘルパーＳネコフード)
+헬퍼Ｓ 고양이 메일(ヘルパーＳネコメイル)\</t>
   </si>
   <si>
     <t>トレニャーの依頼1</t>
@@ -1486,7 +1482,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-オオ筒ドングリ</t>
+큰 통 도토리(オオ筒ドングリ)</t>
   </si>
   <si>
     <t>トレニャーの依頼2</t>
@@ -1499,7 +1495,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-トンガリドングリ</t>
+톤가리도토리(トンガリドングリ)</t>
   </si>
   <si>
     <t>トレニャーの依頼3</t>
@@ -1512,7 +1508,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-アイルー茶釜</t>
+아이루 차솥(アイルー茶釜)</t>
   </si>
   <si>
     <t>ネコートの依頼1</t>
@@ -1525,9 +1521,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX溶岩竜チケット
+EX용암룡 티켓(EX溶岩竜チケット)
 장비개방
-EXラヴァシリーズ</t>
+EX라바 시리즈(EXラヴァシリーズ)</t>
   </si>
   <si>
     <t>ネコートの依頼2</t>
@@ -1540,9 +1536,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX轟竜チケット
+EX굉룡 티켓(EX轟竜チケット)
 장비개방
-EXレックスシリーズ</t>
+EX렉스 시리즈(EXレックスシリーズ)</t>
   </si>
   <si>
     <t>ネコートの依頼3</t>
@@ -1555,11 +1551,11 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX轟竜チケットS
+EX굉룡 티켓Ｓ(EX轟竜チケットＳ)
 장비개방
-EXレックスSシリーズ
+EX렉스Ｓ 시리즈(EXレックスＳシリーズ)
 오토모 장비개방
-ネコートさんのコート</t>
+네코트씨의 코트(ネコートさんのコート)</t>
   </si>
   <si>
     <t>ネコートの依頼4</t>
@@ -1572,7 +1568,7 @@
   </si>
   <si>
     <t>오토모 장비개방
-ネコートさん厚コート</t>
+오코토씨의 두꺼운 코트(ネコートさん厚コート)</t>
   </si>
   <si>
     <t>ポッケ村の看板娘の依頼</t>
@@ -1584,10 +1580,10 @@
     <t>집회소★5 빠른 신룡의 수렵피로(疾き迅竜の狩猟披露)</t>
   </si>
   <si>
-    <t>식재_x000D_
-ユキヤマツタケ
+    <t>식재
+설산 송이버섯(ユキヤマツタケ)
 수기개방
-大挑発LV2</t>
+대도발LV2(大挑発LV2)</t>
   </si>
   <si>
     <t>カリスマ美容師ネコの依頼1</t>
@@ -1599,8 +1595,8 @@
     <t>집회소★3 패션 작렬☆궁극 아프로(パッション炸裂☆究極アフロ)</t>
   </si>
   <si>
-    <t>푸기의 옷_x000D_
-ひよっこアフロ</t>
+    <t>푸기의 옷
+애송이 아프로(ひよっこアフロ)</t>
   </si>
   <si>
     <t>カリスマ美容師ネコの依頼2</t>
@@ -1612,9 +1608,6 @@
     <t>G★2 부딪혀라 삶☆아프로 소울(ぶつけろ生き様☆アフロソウル)</t>
   </si>
   <si>
-    <t>ルームサービス変更可能</t>
-  </si>
-  <si>
     <t>さすらいのコックの依頼1</t>
   </si>
   <si>
@@ -1625,9 +1618,9 @@
   </si>
   <si>
     <t>식재
-モグモガーリック
-푸기의 옷_x000D_
-魅惑のピンク</t>
+모가모갈릭(モグモガーリック)
+푸기의 옷
+매혹의 핑크(魅惑のピンク)</t>
   </si>
   <si>
     <t>さすらいのコックの依頼2</t>
@@ -1639,8 +1632,8 @@
     <t>G★1 앗뜨앗뜨 사막의 순해수렵(アツアツ砂漠の盾蟹狩猟)</t>
   </si>
   <si>
-    <t>식재_x000D_
-エンペラーセロリ</t>
+    <t>식재
+엠페러 셀러리(エンペラーセロリ)</t>
   </si>
   <si>
     <t>工房のばあちゃんの依頼1</t>
@@ -1653,7 +1646,7 @@
   </si>
   <si>
     <t>장비개방
-英雄の双刃</t>
+영웅의 쌍인(英雄の双刃)</t>
   </si>
   <si>
     <t>工房のばあちゃんの依頼2</t>
@@ -1667,11 +1660,11 @@
   </si>
   <si>
     <t>입수
-七色たんぽぽ x10
+일곱 빛깔 민들레 x10(七色たんぽぽ x10)
 장비개방
-EXザザミシリーズ_x000D_
-EXギザミシリーズ_x000D_
-EXブランゴシリーズ</t>
+EX자자미 시리즈(EXザザミシリーズ)
+EX기자미 시리즈(EXギザミシリーズ)
+EX블랑고 시리즈(EXブランゴシリーズ)</t>
   </si>
   <si>
     <t>工房のばあちゃんの依頼3</t>
@@ -1696,7 +1689,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX老山龍チケット</t>
+EX노산룡 티켓(EX老山龍チケット)</t>
   </si>
   <si>
     <t>チャチャの依頼1</t>
@@ -1709,8 +1702,8 @@
   </si>
   <si>
     <t>장비개방
-奇面案山子_x000D_
-棍ガリアチャチャ</t>
+기면 허수아비(奇面案山子)
+곤 가리아챠챠(棍ガリアチャチャ)</t>
   </si>
   <si>
     <t>チャチャの依頼2</t>
@@ -1723,12 +1716,12 @@
   </si>
   <si>
     <t>오토모 장비개방
-怪鳥のクックック_x000D_
-どんぐりのお面_x000D_
-オレチャマの一張羅_x000D_
-大猪のドッドッド_x000D_
-カニ爪のお面_x000D_
-ワガハイのナイスな蓑</t>
+괴조의 쿡쿡쿡(怪鳥のクックック)
+도토리 탈(どんぐりのお面)
+이몸의 단벌 옷(オレチャマの一張羅)
+큰 맷돼지의 도도도(大猪のドッドッド)
+게 발톱 탈(カニ爪のお面)
+본인의 나이스한 도롱이(ワガハイのナイスな蓑)</t>
   </si>
   <si>
     <t>チャチャの依頼3</t>
@@ -1741,9 +1734,9 @@
   </si>
   <si>
     <t>오토모 장비개방
-最高のお面
-수기개방_x000D_
-震怒竜怨斬LV3</t>
+최고의 탈(最高のお面)
+수기개방
+진노용원참LV3(震怒竜怨斬LV3)</t>
   </si>
   <si>
     <t>チャチャの依頼4</t>
@@ -1756,12 +1749,12 @@
   </si>
   <si>
     <t>오토모 장비개방
-大怪鳥のクックック_x000D_
-どんぐりの奇面_x000D_
-オレチャマの天晴れ着_x000D_
-巨大猪のドッドッド_x000D_
-カニ爪の奇面_x000D_
-ワガハイのナイス大蓑</t>
+대괴조의 쿡쿡쿡(大怪鳥のクックック)
+이상한 도토리 탈(どんぐりの奇面)
+이몸의 훌륭한 옷(オレチャマの天晴れ着)
+거대 맷돼지의 도도도(巨大猪のドッドッド)
+이상한 게 발톱 탈(カニ爪の奇面)
+본인의 나이스한 큰 도롱이(ワガハイのナイス大蓑)</t>
   </si>
   <si>
     <t>チャチャの依頼5</t>
@@ -1774,11 +1767,11 @@
   </si>
   <si>
     <t>퀘스트 보수
-奇面な仮面
+기면한 가면(奇面な仮面)
 장비개방
-ニクヤキ銃槍カヤンチャスリンガ
+고기구이 총창 카얀챠스링가(ニクヤキ銃槍カヤンチャスリンガ)
 오토모 장비개방
-極上のお面</t>
+극상의 탈(極上のお面)</t>
   </si>
   <si>
     <t>ギルドマネージャーの依頼1</t>
@@ -1791,7 +1784,7 @@
   </si>
   <si>
     <t>장비개방
-ギルドガード蒼シリーズ</t>
+길드가드 창 시리즈(ギルドガード蒼シリーズ)</t>
   </si>
   <si>
     <t>ギルドマネージャーの依頼2</t>
@@ -1804,7 +1797,7 @@
   </si>
   <si>
     <t>장비개방
-ギルドガード紅シリーズ</t>
+길드가드 홍 시리즈(ギルドガード紅シリーズ)</t>
   </si>
   <si>
     <t>ギルドマネージャーの依頼3</t>
@@ -1817,8 +1810,8 @@
   </si>
   <si>
     <t>장비개방
-Ｇ・ガードＸ蒼シリーズ_x000D_
-Ｇ・ガードＸ紅シリーズ</t>
+Ｇ・가드Ｘ창 시리즈(Ｇ・ガードＸ蒼シリーズ)
+Ｇ・가드Ｘ홍 시리즈(Ｇ・ガードＸ紅シリーズ)</t>
   </si>
   <si>
     <t>유쿠모 마을(ユクモ村)</t>
@@ -1900,6 +1893,10 @@
     <t>마을★3 로아루도로스를 수렵해라!(ロアルドロスを狩猟せよ！)</t>
   </si>
   <si>
+    <t>입수_x000D_
+龍歴院ポイント500pts</t>
+  </si>
+  <si>
     <t>ユクモ村の村長の依頼4</t>
   </si>
   <si>
@@ -2293,6 +2290,9 @@
   </si>
   <si>
     <t>마을★3 엿차! 버섯납품입니다요!(ほいっ！キノコ納品ですよ！)</t>
+  </si>
+  <si>
+    <t>ルームサービス変更可能</t>
   </si>
   <si>
     <t>モガの村の看板娘の依頼2</t>
@@ -3251,8 +3251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D83" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="C119" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4808,7 +4808,7 @@
         <v>362</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>363</v>
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="30">
@@ -4816,16 +4816,16 @@
         <v>351</v>
       </c>
       <c r="B92" t="s">
+        <v>363</v>
+      </c>
+      <c r="C92" t="s">
         <v>364</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>365</v>
       </c>
-      <c r="D92" t="s">
+      <c r="E92" s="1" t="s">
         <v>366</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="75">
@@ -4833,16 +4833,16 @@
         <v>351</v>
       </c>
       <c r="B93" t="s">
+        <v>367</v>
+      </c>
+      <c r="C93" t="s">
         <v>368</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>369</v>
       </c>
-      <c r="D93" t="s">
+      <c r="E93" s="1" t="s">
         <v>370</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="30">
@@ -4850,16 +4850,16 @@
         <v>351</v>
       </c>
       <c r="B94" t="s">
+        <v>371</v>
+      </c>
+      <c r="C94" t="s">
         <v>372</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>373</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="75">
@@ -4867,16 +4867,16 @@
         <v>351</v>
       </c>
       <c r="B95" t="s">
+        <v>375</v>
+      </c>
+      <c r="C95" t="s">
         <v>376</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>377</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="105">
@@ -4884,16 +4884,16 @@
         <v>351</v>
       </c>
       <c r="B96" t="s">
+        <v>379</v>
+      </c>
+      <c r="C96" t="s">
         <v>380</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="105">
@@ -4901,16 +4901,16 @@
         <v>351</v>
       </c>
       <c r="B97" t="s">
+        <v>383</v>
+      </c>
+      <c r="C97" t="s">
         <v>384</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>385</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="105">
@@ -4918,16 +4918,16 @@
         <v>351</v>
       </c>
       <c r="B98" t="s">
+        <v>387</v>
+      </c>
+      <c r="C98" t="s">
         <v>388</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>389</v>
       </c>
-      <c r="D98" t="s">
+      <c r="E98" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="30">
@@ -4935,16 +4935,16 @@
         <v>351</v>
       </c>
       <c r="B99" t="s">
+        <v>391</v>
+      </c>
+      <c r="C99" t="s">
         <v>392</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>393</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30">
@@ -4952,16 +4952,16 @@
         <v>351</v>
       </c>
       <c r="B100" t="s">
+        <v>395</v>
+      </c>
+      <c r="C100" t="s">
         <v>396</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>397</v>
       </c>
-      <c r="D100" t="s">
+      <c r="E100" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30">
@@ -4969,16 +4969,16 @@
         <v>351</v>
       </c>
       <c r="B101" t="s">
+        <v>399</v>
+      </c>
+      <c r="C101" t="s">
         <v>400</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>401</v>
       </c>
-      <c r="D101" t="s">
+      <c r="E101" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="60">
@@ -4986,16 +4986,16 @@
         <v>351</v>
       </c>
       <c r="B102" t="s">
+        <v>403</v>
+      </c>
+      <c r="C102" t="s">
         <v>404</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>405</v>
       </c>
-      <c r="D102" t="s">
+      <c r="E102" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="60">
@@ -5003,16 +5003,16 @@
         <v>351</v>
       </c>
       <c r="B103" t="s">
+        <v>407</v>
+      </c>
+      <c r="C103" t="s">
         <v>408</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>409</v>
       </c>
-      <c r="D103" t="s">
+      <c r="E103" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="90">
@@ -5020,16 +5020,16 @@
         <v>351</v>
       </c>
       <c r="B104" t="s">
+        <v>411</v>
+      </c>
+      <c r="C104" t="s">
         <v>412</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>413</v>
       </c>
-      <c r="D104" t="s">
+      <c r="E104" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30">
@@ -5037,16 +5037,16 @@
         <v>351</v>
       </c>
       <c r="B105" t="s">
+        <v>415</v>
+      </c>
+      <c r="C105" t="s">
         <v>416</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>417</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="60">
@@ -5054,16 +5054,16 @@
         <v>351</v>
       </c>
       <c r="B106" t="s">
+        <v>419</v>
+      </c>
+      <c r="C106" t="s">
         <v>420</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>421</v>
       </c>
-      <c r="D106" t="s">
+      <c r="E106" s="1" t="s">
         <v>422</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30">
@@ -5071,16 +5071,16 @@
         <v>351</v>
       </c>
       <c r="B107" t="s">
+        <v>423</v>
+      </c>
+      <c r="C107" t="s">
         <v>424</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>425</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E107" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -5088,16 +5088,16 @@
         <v>351</v>
       </c>
       <c r="B108" t="s">
+        <v>427</v>
+      </c>
+      <c r="C108" t="s">
         <v>428</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>429</v>
       </c>
-      <c r="D108" t="s">
-        <v>430</v>
-      </c>
       <c r="E108" t="s">
-        <v>431</v>
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="60">
@@ -5105,16 +5105,16 @@
         <v>351</v>
       </c>
       <c r="B109" t="s">
+        <v>430</v>
+      </c>
+      <c r="C109" t="s">
+        <v>431</v>
+      </c>
+      <c r="D109" t="s">
         <v>432</v>
       </c>
-      <c r="C109" t="s">
+      <c r="E109" s="1" t="s">
         <v>433</v>
-      </c>
-      <c r="D109" t="s">
-        <v>434</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="30">
@@ -5122,16 +5122,16 @@
         <v>351</v>
       </c>
       <c r="B110" t="s">
+        <v>434</v>
+      </c>
+      <c r="C110" t="s">
+        <v>435</v>
+      </c>
+      <c r="D110" t="s">
         <v>436</v>
       </c>
-      <c r="C110" t="s">
+      <c r="E110" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="D110" t="s">
-        <v>438</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="30">
@@ -5139,16 +5139,16 @@
         <v>351</v>
       </c>
       <c r="B111" t="s">
+        <v>438</v>
+      </c>
+      <c r="C111" t="s">
+        <v>439</v>
+      </c>
+      <c r="D111" t="s">
         <v>440</v>
       </c>
-      <c r="C111" t="s">
+      <c r="E111" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="D111" t="s">
-        <v>442</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="90">
@@ -5156,16 +5156,16 @@
         <v>351</v>
       </c>
       <c r="B112" t="s">
+        <v>442</v>
+      </c>
+      <c r="C112" t="s">
+        <v>443</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="C112" t="s">
+      <c r="E112" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -5173,16 +5173,16 @@
         <v>351</v>
       </c>
       <c r="B113" t="s">
+        <v>446</v>
+      </c>
+      <c r="C113" t="s">
+        <v>447</v>
+      </c>
+      <c r="D113" t="s">
         <v>448</v>
       </c>
-      <c r="C113" t="s">
+      <c r="E113" t="s">
         <v>449</v>
-      </c>
-      <c r="D113" t="s">
-        <v>450</v>
-      </c>
-      <c r="E113" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="30">
@@ -5190,16 +5190,16 @@
         <v>351</v>
       </c>
       <c r="B114" t="s">
+        <v>450</v>
+      </c>
+      <c r="C114" t="s">
+        <v>451</v>
+      </c>
+      <c r="D114" t="s">
         <v>452</v>
       </c>
-      <c r="C114" t="s">
+      <c r="E114" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="D114" t="s">
-        <v>454</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="45">
@@ -5207,16 +5207,16 @@
         <v>351</v>
       </c>
       <c r="B115" t="s">
+        <v>454</v>
+      </c>
+      <c r="C115" t="s">
+        <v>455</v>
+      </c>
+      <c r="D115" t="s">
         <v>456</v>
       </c>
-      <c r="C115" t="s">
+      <c r="E115" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="D115" t="s">
-        <v>458</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="105">
@@ -5224,16 +5224,16 @@
         <v>351</v>
       </c>
       <c r="B116" t="s">
+        <v>458</v>
+      </c>
+      <c r="C116" t="s">
+        <v>459</v>
+      </c>
+      <c r="D116" t="s">
         <v>460</v>
       </c>
-      <c r="C116" t="s">
+      <c r="E116" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="D116" t="s">
-        <v>462</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="60">
@@ -5241,16 +5241,16 @@
         <v>351</v>
       </c>
       <c r="B117" t="s">
+        <v>462</v>
+      </c>
+      <c r="C117" t="s">
+        <v>463</v>
+      </c>
+      <c r="D117" t="s">
         <v>464</v>
       </c>
-      <c r="C117" t="s">
+      <c r="E117" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="D117" t="s">
-        <v>466</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="105">
@@ -5258,16 +5258,16 @@
         <v>351</v>
       </c>
       <c r="B118" t="s">
+        <v>466</v>
+      </c>
+      <c r="C118" t="s">
+        <v>467</v>
+      </c>
+      <c r="D118" t="s">
         <v>468</v>
       </c>
-      <c r="C118" t="s">
+      <c r="E118" s="1" t="s">
         <v>469</v>
-      </c>
-      <c r="D118" t="s">
-        <v>470</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="90">
@@ -5275,16 +5275,16 @@
         <v>351</v>
       </c>
       <c r="B119" t="s">
+        <v>470</v>
+      </c>
+      <c r="C119" t="s">
+        <v>471</v>
+      </c>
+      <c r="D119" t="s">
         <v>472</v>
       </c>
-      <c r="C119" t="s">
+      <c r="E119" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="D119" t="s">
-        <v>474</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30">
@@ -5292,16 +5292,16 @@
         <v>351</v>
       </c>
       <c r="B120" t="s">
+        <v>474</v>
+      </c>
+      <c r="C120" t="s">
+        <v>475</v>
+      </c>
+      <c r="D120" t="s">
         <v>476</v>
       </c>
-      <c r="C120" t="s">
+      <c r="E120" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="D120" t="s">
-        <v>478</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30">
@@ -5309,16 +5309,16 @@
         <v>351</v>
       </c>
       <c r="B121" t="s">
+        <v>478</v>
+      </c>
+      <c r="C121" t="s">
+        <v>479</v>
+      </c>
+      <c r="D121" t="s">
         <v>480</v>
       </c>
-      <c r="C121" t="s">
+      <c r="E121" s="1" t="s">
         <v>481</v>
-      </c>
-      <c r="D121" t="s">
-        <v>482</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="45">
@@ -5326,565 +5326,565 @@
         <v>351</v>
       </c>
       <c r="B122" t="s">
+        <v>482</v>
+      </c>
+      <c r="C122" t="s">
+        <v>483</v>
+      </c>
+      <c r="D122" t="s">
         <v>484</v>
       </c>
-      <c r="C122" t="s">
+      <c r="E122" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="D122" t="s">
-        <v>486</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="390">
       <c r="A123" t="s">
+        <v>486</v>
+      </c>
+      <c r="B123" t="s">
+        <v>487</v>
+      </c>
+      <c r="C123" t="s">
         <v>488</v>
       </c>
-      <c r="B123" t="s">
+      <c r="D123" t="s">
         <v>489</v>
       </c>
-      <c r="C123" t="s">
+      <c r="E123" s="1" t="s">
         <v>490</v>
-      </c>
-      <c r="D123" t="s">
-        <v>491</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="30">
       <c r="A124" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B124" t="s">
+        <v>491</v>
+      </c>
+      <c r="C124" t="s">
+        <v>492</v>
+      </c>
+      <c r="D124" t="s">
         <v>493</v>
       </c>
-      <c r="C124" t="s">
+      <c r="E124" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="D124" t="s">
-        <v>495</v>
-      </c>
-      <c r="E124" s="1" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="90">
       <c r="A125" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B125" t="s">
+        <v>495</v>
+      </c>
+      <c r="C125" t="s">
+        <v>496</v>
+      </c>
+      <c r="D125" t="s">
         <v>497</v>
       </c>
-      <c r="C125" t="s">
+      <c r="E125" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="D125" t="s">
-        <v>499</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="30">
       <c r="A126" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B126" t="s">
+        <v>499</v>
+      </c>
+      <c r="C126" t="s">
+        <v>500</v>
+      </c>
+      <c r="D126" t="s">
         <v>501</v>
       </c>
-      <c r="C126" t="s">
+      <c r="E126" s="1" t="s">
         <v>502</v>
-      </c>
-      <c r="D126" t="s">
-        <v>503</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30">
       <c r="A127" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B127" t="s">
+        <v>503</v>
+      </c>
+      <c r="C127" t="s">
         <v>504</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>505</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="60">
       <c r="A128" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B128" t="s">
+        <v>507</v>
+      </c>
+      <c r="C128" t="s">
         <v>508</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>509</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" s="1" t="s">
         <v>510</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30">
       <c r="A129" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B129" t="s">
+        <v>511</v>
+      </c>
+      <c r="C129" t="s">
         <v>512</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
         <v>513</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" s="1" t="s">
         <v>514</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="90">
       <c r="A130" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B130" t="s">
+        <v>515</v>
+      </c>
+      <c r="C130" t="s">
         <v>516</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>517</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="90">
       <c r="A131" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B131" t="s">
+        <v>519</v>
+      </c>
+      <c r="C131" t="s">
         <v>520</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>521</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131" s="1" t="s">
         <v>522</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="75">
       <c r="A132" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B132" t="s">
+        <v>523</v>
+      </c>
+      <c r="C132" t="s">
         <v>524</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>525</v>
       </c>
-      <c r="D132" t="s">
+      <c r="E132" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="75">
       <c r="A133" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B133" t="s">
+        <v>527</v>
+      </c>
+      <c r="C133" t="s">
         <v>528</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>529</v>
       </c>
-      <c r="D133" t="s">
+      <c r="E133" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="30">
       <c r="A134" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B134" t="s">
+        <v>531</v>
+      </c>
+      <c r="C134" t="s">
         <v>532</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>533</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45">
       <c r="A135" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B135" t="s">
+        <v>535</v>
+      </c>
+      <c r="C135" t="s">
         <v>536</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45">
       <c r="A136" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B136" t="s">
+        <v>539</v>
+      </c>
+      <c r="C136" t="s">
         <v>540</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>541</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="45">
       <c r="A137" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B137" t="s">
+        <v>543</v>
+      </c>
+      <c r="C137" t="s">
         <v>544</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>545</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45">
       <c r="A138" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B138" t="s">
+        <v>547</v>
+      </c>
+      <c r="C138" t="s">
         <v>548</v>
       </c>
-      <c r="C138" t="s">
+      <c r="D138" t="s">
         <v>549</v>
       </c>
-      <c r="D138" t="s">
+      <c r="E138" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="60">
       <c r="A139" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B139" t="s">
+        <v>551</v>
+      </c>
+      <c r="C139" t="s">
         <v>552</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
         <v>553</v>
       </c>
-      <c r="D139" t="s">
+      <c r="E139" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="60">
       <c r="A140" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B140" t="s">
+        <v>555</v>
+      </c>
+      <c r="C140" t="s">
         <v>556</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
         <v>557</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" s="1" t="s">
         <v>558</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="60">
       <c r="A141" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B141" t="s">
+        <v>559</v>
+      </c>
+      <c r="C141" t="s">
         <v>560</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>561</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" s="1" t="s">
         <v>562</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30">
       <c r="A142" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B142" t="s">
+        <v>563</v>
+      </c>
+      <c r="C142" t="s">
         <v>564</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>565</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" s="1" t="s">
         <v>566</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30">
       <c r="A143" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B143" t="s">
+        <v>567</v>
+      </c>
+      <c r="C143" t="s">
         <v>568</v>
       </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
         <v>569</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" s="1" t="s">
         <v>570</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30">
       <c r="A144" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B144" t="s">
+        <v>571</v>
+      </c>
+      <c r="C144" t="s">
         <v>572</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>573</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30">
       <c r="A145" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B145" t="s">
+        <v>575</v>
+      </c>
+      <c r="C145" t="s">
         <v>576</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>577</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="30">
       <c r="A146" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B146" t="s">
+        <v>579</v>
+      </c>
+      <c r="C146" t="s">
         <v>580</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>581</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" s="1" t="s">
         <v>582</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30">
       <c r="A147" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B147" t="s">
+        <v>583</v>
+      </c>
+      <c r="C147" t="s">
         <v>584</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="E147" s="1" t="s">
         <v>586</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="30">
       <c r="A148" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B148" t="s">
+        <v>587</v>
+      </c>
+      <c r="C148" t="s">
         <v>588</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>589</v>
       </c>
-      <c r="D148" t="s">
+      <c r="E148" s="1" t="s">
         <v>590</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="30">
       <c r="A149" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B149" t="s">
+        <v>591</v>
+      </c>
+      <c r="C149" t="s">
         <v>592</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>593</v>
       </c>
-      <c r="D149" t="s">
+      <c r="E149" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30">
       <c r="A150" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B150" t="s">
+        <v>595</v>
+      </c>
+      <c r="C150" t="s">
         <v>596</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>597</v>
       </c>
-      <c r="D150" t="s">
+      <c r="E150" s="1" t="s">
         <v>598</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="90">
       <c r="A151" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B151" t="s">
+        <v>599</v>
+      </c>
+      <c r="C151" t="s">
         <v>600</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" t="s">
         <v>601</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" s="1" t="s">
         <v>602</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="45">
       <c r="A152" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B152" t="s">
+        <v>603</v>
+      </c>
+      <c r="C152" t="s">
         <v>604</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="D152" s="1" t="s">
+      <c r="E152" s="1" t="s">
         <v>606</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="30">
       <c r="A153" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B153" t="s">
+        <v>607</v>
+      </c>
+      <c r="C153" t="s">
         <v>608</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>609</v>
       </c>
-      <c r="D153" t="s">
+      <c r="E153" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B154" t="s">
+        <v>611</v>
+      </c>
+      <c r="C154" t="s">
         <v>612</v>
       </c>
-      <c r="C154" t="s">
+      <c r="D154" t="s">
         <v>613</v>
       </c>
-      <c r="D154" t="s">
+      <c r="E154" t="s">
         <v>614</v>
-      </c>
-      <c r="E154" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="75">
       <c r="A155" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B155" t="s">
         <v>615</v>
@@ -5901,7 +5901,7 @@
     </row>
     <row r="156" spans="1:5" ht="75">
       <c r="A156" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B156" t="s">
         <v>619</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="157" spans="1:5" ht="75">
       <c r="A157" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B157" t="s">
         <v>623</v>
@@ -5935,7 +5935,7 @@
     </row>
     <row r="158" spans="1:5">
       <c r="A158" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B158" t="s">
         <v>627</v>
@@ -5947,12 +5947,12 @@
         <v>629</v>
       </c>
       <c r="E158" t="s">
-        <v>431</v>
+        <v>614</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="60">
       <c r="A159" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B159" t="s">
         <v>630</v>
@@ -5969,7 +5969,7 @@
     </row>
     <row r="160" spans="1:5" ht="30">
       <c r="A160" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B160" t="s">
         <v>634</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="161" spans="1:5" ht="30">
       <c r="A161" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B161" t="s">
         <v>638</v>
@@ -6003,7 +6003,7 @@
     </row>
     <row r="162" spans="1:5" ht="30">
       <c r="A162" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B162" t="s">
         <v>642</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="163" spans="1:5">
       <c r="A163" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B163" t="s">
         <v>646</v>
@@ -6032,12 +6032,12 @@
         <v>648</v>
       </c>
       <c r="E163" t="s">
-        <v>431</v>
+        <v>614</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="30">
       <c r="A164" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B164" t="s">
         <v>649</v>
@@ -6054,7 +6054,7 @@
     </row>
     <row r="165" spans="1:5" ht="60">
       <c r="A165" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B165" t="s">
         <v>653</v>
@@ -6071,7 +6071,7 @@
     </row>
     <row r="166" spans="1:5" ht="60">
       <c r="A166" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B166" t="s">
         <v>657</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="167" spans="1:5" ht="30">
       <c r="A167" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B167" t="s">
         <v>661</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="168" spans="1:5" ht="30">
       <c r="A168" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B168" t="s">
         <v>665</v>
@@ -6122,7 +6122,7 @@
     </row>
     <row r="169" spans="1:5" ht="30">
       <c r="A169" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B169" t="s">
         <v>669</v>
@@ -6139,7 +6139,7 @@
     </row>
     <row r="170" spans="1:5" ht="60">
       <c r="A170" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B170" t="s">
         <v>673</v>
@@ -6156,7 +6156,7 @@
     </row>
     <row r="171" spans="1:5" ht="60">
       <c r="A171" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B171" t="s">
         <v>677</v>
@@ -6173,7 +6173,7 @@
     </row>
     <row r="172" spans="1:5" ht="30">
       <c r="A172" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B172" t="s">
         <v>681</v>
@@ -6190,7 +6190,7 @@
     </row>
     <row r="173" spans="1:5" ht="60">
       <c r="A173" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B173" t="s">
         <v>685</v>
@@ -6207,7 +6207,7 @@
     </row>
     <row r="174" spans="1:5" ht="30">
       <c r="A174" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B174" t="s">
         <v>689</v>
@@ -6224,7 +6224,7 @@
     </row>
     <row r="175" spans="1:5" ht="60">
       <c r="A175" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B175" t="s">
         <v>693</v>
@@ -6241,7 +6241,7 @@
     </row>
     <row r="176" spans="1:5" ht="30">
       <c r="A176" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B176" t="s">
         <v>697</v>
@@ -6258,7 +6258,7 @@
     </row>
     <row r="177" spans="1:5" ht="30">
       <c r="A177" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B177" t="s">
         <v>701</v>
@@ -6275,7 +6275,7 @@
     </row>
     <row r="178" spans="1:5" ht="75">
       <c r="A178" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B178" t="s">
         <v>705</v>
@@ -6292,7 +6292,7 @@
     </row>
     <row r="179" spans="1:5" ht="60">
       <c r="A179" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B179" t="s">
         <v>709</v>
@@ -6309,7 +6309,7 @@
     </row>
     <row r="180" spans="1:5" ht="60">
       <c r="A180" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B180" t="s">
         <v>713</v>
@@ -6326,7 +6326,7 @@
     </row>
     <row r="181" spans="1:5" ht="30">
       <c r="A181" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B181" t="s">
         <v>717</v>
@@ -6343,7 +6343,7 @@
     </row>
     <row r="182" spans="1:5" ht="60">
       <c r="A182" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B182" t="s">
         <v>721</v>
@@ -6360,7 +6360,7 @@
     </row>
     <row r="183" spans="1:5" ht="60">
       <c r="A183" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B183" t="s">
         <v>725</v>
@@ -6377,7 +6377,7 @@
     </row>
     <row r="184" spans="1:5" ht="60">
       <c r="A184" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B184" t="s">
         <v>729</v>

</xml_diff>

<commit_message>
requestQuest: Name translation of equipment and foodstuffs to be opened.(~ユクモ Town)
</commit_message>
<xml_diff>
--- a/request.xlsx
+++ b/request.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="776">
   <si>
     <t>town</t>
   </si>
@@ -433,7 +433,7 @@
     <t>집회소★7 초☆메모장 ~천인룡포획편~(超☆メモ帳～千刃竜捕獲編～)</t>
   </si>
   <si>
-    <t>룸서비스 변경가능(ルームサービス変更可能)</t>
+    <t>룸서비스 변경가능</t>
   </si>
   <si>
     <t>キャラバンの看板娘の依頼4</t>
@@ -1827,30 +1827,30 @@
   </si>
   <si>
     <t>장비개방
-アークRシリーズ_x000D_
-アーティアRシリーズ_x000D_
-アカムトRシリーズ_x000D_
-アロイRシリーズ_x000D_
-インゴットRシリーズ_x000D_
-エスカドラRシリーズ_x000D_
-ギザミRシリーズ_x000D_
-キリンRシリーズ_x000D_
-クシャナRシリーズ_x000D_
-グリードRシリーズ_x000D_
-ゲリョスRシリーズ_x000D_
-ゴアRシリーズ_x000D_
-S・ソルRシリーズ_x000D_
-ザザミRシリーズ_x000D_
-ダマスクRシリーズ_x000D_
-タロスRシリーズ_x000D_
-デスギアRシリーズ_x000D_
-ハンターRシリーズ_x000D_
-フィリアRシリーズ_x000D_
-フルフルRシリーズ_x000D_
-ラギアRシリーズ_x000D_
-ルドロスRシリーズ_x000D_
-レイアRシリーズ_x000D_
-レウスRシリーズ_x000D_
+아크R 시리즈(アークRシリーズ)
+아티아R 시리즈(アーティアRシリーズ)
+아캄토R 시리즈(アカムトRシリーズ)
+아로이R 시리즈(アロイRシリーズ)
+잉곳R 시리즈(インゴットRシリーズ)
+에스카드라R 시리즈(エスカドラRシリーズ)
+기자미R 시리즈(ギザミRシリーズ)
+키린R 시리즈(キリンRシリーズ)
+크샤나R 시리즈(クシャナRシリーズ)
+그리드R 시리즈(グリードRシリーズ)
+게료스R 시리즈(ゲリョスRシリーズ)
+고어R 시리즈(ゴアRシリーズ)
+S・솔R 시리즈(S・ソルRシリーズ)
+자자미R 시리즈(ザザミRシリーズ)
+다마스크R 시리즈(ダマスクRシリーズ)
+타로스R 시리즈(タロスRシリーズ)
+데스기어R 시리즈(デスギアRシリーズ)
+헌터R 시리즈(ハンターRシリーズ)
+필리아R 시리즈(フィリアRシリーズ)
+푸르푸르R 시리즈(フルフルRシリーズ)
+라기아R 시리즈(ラギアRシリーズ)
+루도로스R 시리즈(ルドロスRシリーズ)
+레이아R 시리즈(レイアRシリーズ)
+レウスRシリーズ
 レックスRシリーズ</t>
   </si>
   <si>
@@ -1863,8 +1863,8 @@
     <t>마을★2 계류의 쟈기노스 퇴치(渓流のジャギィノス退治)</t>
   </si>
   <si>
-    <t>입수_x000D_
-ユクモ村の村貢献度100pts</t>
+    <t>입수
+유쿠모 마을의 마을 공헌도 100pts(ユクモ村の村貢献度100pts)</t>
   </si>
   <si>
     <t>ユクモ村の村長の依頼2</t>
@@ -1877,11 +1877,11 @@
   </si>
   <si>
     <t>장비개방
-ユクモノシリーズ
+유쿠모노 시리즈(ユクモノシリーズ)
 오토모 장비개방
-ユクモノネコ木刀_x000D_
-ユクモノネコカサ_x000D_
-ユクモノネコドウギ</t>
+유쿠모노 고양이 목도(ユクモノネコ木刀)
+유쿠모노 고양이 우산(ユクモノネコカサ)
+유쿠모노 고양이 동의(ユクモノネコドウギ)</t>
   </si>
   <si>
     <t>ユクモ村の村長の依頼3</t>
@@ -1893,10 +1893,6 @@
     <t>마을★3 로아루도로스를 수렵해라!(ロアルドロスを狩猟せよ！)</t>
   </si>
   <si>
-    <t>입수_x000D_
-龍歴院ポイント500pts</t>
-  </si>
-  <si>
     <t>ユクモ村の村長の依頼4</t>
   </si>
   <si>
@@ -1907,7 +1903,7 @@
   </si>
   <si>
     <t>입수
-ユクモチケット x2</t>
+유쿠모 티켓 x2(ユクモチケット x2)</t>
   </si>
   <si>
     <t>ユクモ村の村長の依頼5</t>
@@ -1920,9 +1916,9 @@
   </si>
   <si>
     <t>입수
-ユクモチケット x5
-수기개방_x000D_
-アクセルシャワーLV2</t>
+유쿠모 티켓 x5(ユクモチケット x5)
+수기개방
+액셀 샤워LV2(アクセルシャワーLV2)</t>
   </si>
   <si>
     <t>ユクモ村の村長の依頼6</t>
@@ -1935,7 +1931,7 @@
   </si>
   <si>
     <t>입수
-隼刃の羽飾り</t>
+준인의 깃털 장식(隼刃の羽飾り)</t>
   </si>
   <si>
     <t>ユクモ村の村長の依頼7</t>
@@ -1948,11 +1944,11 @@
   </si>
   <si>
     <t>입수
-ユクモチケットG
+유쿠모 티켓 G(ユクモチケットG)
 오토모 장비개방
-ユクモノＸネコ扇子_x000D_
-ユクモノＸネコカサ_x000D_
-ユクモノＸネコドウギ</t>
+유쿠모노Ｘ 고양이 부채(ユクモノＸネコ扇子)
+유쿠모노Ｘ 고양이 우산(ユクモノＸネコカサ)
+유쿠모노Ｘ 고양이 동의(ユクモノＸネコドウギ)</t>
   </si>
   <si>
     <t>ユクモ村の受付嬢の依頼1</t>
@@ -1965,11 +1961,11 @@
   </si>
   <si>
     <t>장비개방
-撫子/桔梗シリーズ
+나데시코/키쿄우 시리즈(撫子/桔梗シリーズ)
 오토모 장비개방
-ユクモノネコ扇子_x000D_
-ニャでしこ【布冠】_x000D_
-ニャでしこ【花衣】</t>
+유쿠모노 고양이 부채(ユクモノネコ扇子)
+냐데시코【포관】(ニャでしこ【布冠】)
+냐데시코【화의】(ニャでしこ【花衣】)</t>
   </si>
   <si>
     <t>ユクモ村の受付嬢の依頼2</t>
@@ -1982,10 +1978,10 @@
   </si>
   <si>
     <t>장비개방
-撫子・雅/桔梗・雅シリーズ
+나데시코・아/키쿄우・아 시리즈(撫子・雅/桔梗・雅シリーズ)
 오토모 장비개방
-ニャでしこ雅【布冠】_x000D_
-ニャでしこ雅【花衣】</t>
+냐데시코아【포관】(ニャでしこ雅【布冠】)
+냐데시코아【화의】(ニャでしこ雅【花衣】)</t>
   </si>
   <si>
     <t>ユクモ村の看板娘の依頼1</t>
@@ -1998,10 +1994,10 @@
   </si>
   <si>
     <t>장비개방
-撫子・華/桔梗・華シリーズ
+나데시코・화/키쿄우・화 시리즈(撫子・華/桔梗・華シリーズ)
 오토모 장비개방
-ニャでしこ華【布冠】_x000D_
-ニャでしこ華【花衣】</t>
+냐데시코화【포관】(ニャでしこ華【布冠】)
+냐데시코화【화의】(ニャでしこ華【花衣】)</t>
   </si>
   <si>
     <t>ユクモ村の看板娘の依頼2</t>
@@ -2013,8 +2009,8 @@
     <t>G★1 간판 아가씨 셀렉트 : 유군령의 수수(看板娘セレクト：遺群嶺の水獣)</t>
   </si>
   <si>
-    <t>입수_x000D_
-ユクモ村の村貢献度500pts</t>
+    <t>입수
+유쿠모 마을의 마을 공헌도 500pts(ユクモ村の村貢献度500pts)</t>
   </si>
   <si>
     <t>オトモ武具屋の依頼1</t>
@@ -2029,8 +2025,8 @@
   </si>
   <si>
     <t>오토모 장비개방
-マカネコピック_x000D_
-巨大ネコどんぐり</t>
+마카 고양이 피크(マカネコピック)
+거대 고양이 도토리(巨大ネコどんぐり)</t>
   </si>
   <si>
     <t>オトモ武具屋の依頼2</t>
@@ -2043,8 +2039,8 @@
   </si>
   <si>
     <t>오토모 장비개방
-ランポスネコピック_x000D_
-大タルネコハンマー</t>
+란포스 고양이 피크(ランポスネコピック)
+큰 통 고양이 해머(大タルネコハンマー)</t>
   </si>
   <si>
     <t>オトモ武具屋の依頼3</t>
@@ -2057,8 +2053,8 @@
   </si>
   <si>
     <t>오토모 장비개방
-転がし三度笠_x000D_
-転がしマント</t>
+굴림 삿갓(転がし三度笠)
+굴림 망토(転がしマント)</t>
   </si>
   <si>
     <t>オトモ武具屋の依頼4</t>
@@ -2071,8 +2067,8 @@
   </si>
   <si>
     <t>오토모 장비개방
-転々がし三度笠_x000D_
-転々がしマント</t>
+굴림굴림 삿갓(転々がし三度笠)
+굴림굴림 망토(転々がしマント)</t>
   </si>
   <si>
     <t>集会浴場の番台さんの依頼1</t>
@@ -2085,9 +2081,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX雷狼竜チケット
+EX뇌랑룡 티켓(EX雷狼竜チケット)
 장비개방
-EXジンオウシリーズ</t>
+EX진오우가 시리즈(EXジンオウシリーズ)</t>
   </si>
   <si>
     <t>集会浴場の番台さんの依頼2</t>
@@ -2100,9 +2096,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-EX砕竜チケット
+EX 쇄룡 티켓(EX砕竜チケット)
 장비개방
-EXブラキシリーズ</t>
+EX 브라키 시리즈(EXブラキシリーズ)</t>
   </si>
   <si>
     <t>集会浴場の番台さんの依頼3</t>
@@ -2115,9 +2111,9 @@
   </si>
   <si>
     <t>장비개방
-桐花/三葵シリーズ
+동화/삼규 시리즈(桐花/三葵シリーズ)
 수기개방
-蟲纏いLV3</t>
+벌레 두르기LV3(蟲纏いLV3)</t>
   </si>
   <si>
     <t>集会浴場の番台さんの依頼4</t>
@@ -2130,7 +2126,7 @@
   </si>
   <si>
     <t>장비개방
-最高級ユアミシリーズ</t>
+최고급 유아미 시리즈(最高級ユアミシリーズ)</t>
   </si>
   <si>
     <t>モガの村の農場長の依頼1</t>
@@ -2143,7 +2139,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-コシカケダケ</t>
+의자 버섯(コシカケダケ)</t>
   </si>
   <si>
     <t>モガの村の農場長の依頼2</t>
@@ -2156,7 +2152,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-キングサボテン</t>
+킹 선인장(キングサボテン)</t>
   </si>
   <si>
     <t>モガの村の農場長の依頼3</t>
@@ -2169,7 +2165,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-オオモロコシ</t>
+큰 수수(オオモロコシ)</t>
   </si>
   <si>
     <t>モガの村の農場長の依頼4</t>
@@ -2181,8 +2177,8 @@
     <t>마을★9 정글・페로몬(ジャングル・フェロモン)</t>
   </si>
   <si>
-    <t>식재_x000D_
-マスターベーグル</t>
+    <t>식재
+마스터 베이글(マスターベーグル)</t>
   </si>
   <si>
     <t>モガの村長の息子の依頼1</t>
@@ -2195,8 +2191,8 @@
 생고기(生肉) x3</t>
   </si>
   <si>
-    <t>식재_x000D_
-モガニ</t>
+    <t>식재
+모가니(モガニ)</t>
   </si>
   <si>
     <t>モガの村長の息子の依頼2</t>
@@ -2209,7 +2205,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-うなりうねり貝</t>
+으르렁으르렁조개(うなりうねり貝)</t>
   </si>
   <si>
     <t>モガの村長の息子の依頼3</t>
@@ -2222,7 +2218,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-古代鮫の皮</t>
+고대상어의 가죽(古代鮫の皮)</t>
   </si>
   <si>
     <t>モガの村長の息子の依頼4</t>
@@ -2235,7 +2231,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-イチノタチウオ</t>
+가장 뛰어난 갈치(イチノタチウオ)</t>
   </si>
   <si>
     <t>モガの村長の息子の依頼5</t>
@@ -2248,11 +2244,11 @@
   </si>
   <si>
     <t>퀘스트 보수
-大海原の輝石
+대해원의 휘석(大海原の輝石)
 장비개방
-ヴァイキングホーン_x000D_
-ヘリオスＸシリーズ_x000D_
-セレネＸシリーズ</t>
+바이킹 혼(ヴァイキングホーン)
+베리오스Ｘ 시리즈(ヘリオスＸシリーズ)
+셀레네Ｘ 시리즈(セレネＸシリーズ)</t>
   </si>
   <si>
     <t>漁港の女主人の依頼1</t>
@@ -2266,8 +2262,8 @@
 지친정어리(シンドイワシ) x2</t>
   </si>
   <si>
-    <t>식재_x000D_
-モガ大トロ</t>
+    <t>식재
+모가 큰 다랑어(モガ大トロ)</t>
   </si>
   <si>
     <t>漁港の女主人の依頼2</t>
@@ -2279,8 +2275,8 @@
     <t>G★1 강변의 아오아시라 퇴치(川辺のアオアシラ退治)</t>
   </si>
   <si>
-    <t>식재_x000D_
-カタマリアワビ</t>
+    <t>식재
+덩어리 전복(カタマリアワビ)</t>
   </si>
   <si>
     <t>モガの村の看板娘の依頼1</t>
@@ -2292,9 +2288,6 @@
     <t>마을★3 엿차! 버섯납품입니다요!(ほいっ！キノコ納品ですよ！)</t>
   </si>
   <si>
-    <t>ルームサービス変更可能</t>
-  </si>
-  <si>
     <t>モガの村の看板娘の依頼2</t>
   </si>
   <si>
@@ -2305,10 +2298,10 @@
   </si>
   <si>
     <t>장비개방
-スカラーシリーズ
+스칼라 시리즈(スカラーシリーズ)
 오토모 장비개방
-ガイドネコフード_x000D_
-ガイドネコスーツ</t>
+가이드 고양이 후드(ガイドネコフード)
+가이드 고양이 슈트(ガイドネコスーツ)</t>
   </si>
   <si>
     <t>モガの村の看板娘の依頼3</t>
@@ -2321,10 +2314,10 @@
   </si>
   <si>
     <t>장비개방
-スカラーＸシリーズ
+스칼라Ｘ 시리즈(スカラーＸシリーズ)
 오토모 장비개방
-ガイドＸネコフード_x000D_
-ガイドＸネコスーツ</t>
+가이드Ｘ 고양이 후드(ガイドＸネコフード)
+가이드Ｘ 고양이 슈트(ガイドＸネコスーツ)</t>
   </si>
   <si>
     <t>タンジアの港の看板娘の依頼1</t>
@@ -2337,10 +2330,10 @@
   </si>
   <si>
     <t>장비개방
-セイラーシリーズ
+세일러 시리즈(セイラーシリーズ)
 오토모 장비개방
-セイラーネコフード_x000D_
-セイラーネコスーツ</t>
+세일러 고양이 후드(セイラーネコフード)
+세일러 고양이 슈트(セイラーネコスーツ)</t>
   </si>
   <si>
     <t>タンジアの港の看板娘の依頼2</t>
@@ -2365,9 +2358,10 @@
   </si>
   <si>
     <t>장비개방
-セイラーＸシリーズ
+세일러Ｘ 시리즈(セイラーＸシリーズ)
 오토모 장비개방
-セイラーＸネコフードセイラーＸネコスーツ</t>
+세일러Ｘ 고양이 후드(セイラーＸネコフード)_x000D_
+세일러Ｘ 고양이 슈트(セイラーＸネコスーツ)</t>
   </si>
   <si>
     <t>ロックラックの宿屋の依頼</t>
@@ -2380,8 +2374,8 @@
 수수께끼의 뼈(なぞの骨) x5</t>
   </si>
   <si>
-    <t>식재_x000D_
-ロックラックルミ</t>
+    <t>식재
+록락 호두(ロックラックルミ)</t>
   </si>
   <si>
     <t>孤高の教官の依頼</t>
@@ -2393,8 +2387,8 @@
     <t>마을★6 뇌랑룡은 이렇게 울었다(雷狼竜はかく吠えり)</t>
   </si>
   <si>
-    <t>식재_x000D_
-達人ビール</t>
+    <t>식재
+달인 맥주(達人ビール)</t>
   </si>
   <si>
     <t>ぽかぽか島の管理人の依頼1</t>
@@ -2406,8 +2400,8 @@
     <t>마을★2 따끈따끈 죽순 납품(ぽかぽかタケノコ納品)</t>
   </si>
   <si>
-    <t>식재_x000D_
-ツチタケノコ</t>
+    <t>식재
+땅 죽순(ツチタケノコ)</t>
   </si>
   <si>
     <t>ぽかぽか島の管理人の依頼2</t>
@@ -2428,8 +2422,8 @@
     <t>마을★3 순해와 조개와 사냥(盾蟹と貝と狩り)</t>
   </si>
   <si>
-    <t>식재_x000D_
-モガモ貝</t>
+    <t>식재
+모가모 조개(モガモ貝)</t>
   </si>
   <si>
     <t>モガの村の村長の依頼2</t>
@@ -2442,9 +2436,9 @@
   </si>
   <si>
     <t>퀘스트 보수
-大海原の輝石
+대해원의 휘석(大海原の輝石)
 장비개방
-ナバルタスク</t>
+나발타스크(ナバルタスク)</t>
   </si>
   <si>
     <t>ジャンボ村の村長の依頼1</t>
@@ -2459,10 +2453,10 @@
 빙결정 딸기(氷結晶イチゴ) x1</t>
   </si>
   <si>
-    <t>식재_x000D_
-ジャンボウ
-푸기의 옷_x000D_
-はだかの王様</t>
+    <t>식재
+점보우(ジャンボウ)
+푸기의 옷
+벌거벗은 임금님(はだかの王様)</t>
   </si>
   <si>
     <t>ジャンボ村の村長の依頼2</t>
@@ -2475,7 +2469,7 @@
   </si>
   <si>
     <t>입수
-封龍宝剣</t>
+봉룡보검(封龍宝剣)</t>
   </si>
   <si>
     <t>食材屋の女将の依頼1</t>
@@ -2487,8 +2481,8 @@
     <t>집회소★2 식재의 가치는 신선도이다(食材の価値は鮮度なり)</t>
   </si>
   <si>
-    <t>식재_x000D_
-サイコロミート</t>
+    <t>식재
+주사위 고기(サイコロミート)</t>
   </si>
   <si>
     <t>食材屋の女将の依頼2</t>
@@ -2500,8 +2494,8 @@
     <t>마을★7 제철 식재를 채집해주게!(旬な食材を採らせておくれ！)</t>
   </si>
   <si>
-    <t>식재_x000D_
-リュウノテール</t>
+    <t>식재
+용 꼬리(リュウノテール)</t>
   </si>
   <si>
     <t>調合屋のあるじの依頼</t>
@@ -2516,8 +2510,8 @@
 극채색의 체액(極彩色の体液) x1</t>
   </si>
   <si>
-    <t>식재_x000D_
-五穀豊穣米</t>
+    <t>식재
+오곡풍양미(五穀豊穣米)</t>
   </si>
   <si>
     <t>ドンドルマの道具屋の依頼1</t>
@@ -2529,10 +2523,10 @@
     <t>집회소★6 환상의 핫플?(幻のハップル？)</t>
   </si>
   <si>
-    <t>식재_x000D_
-ハップルアップル
-푸기의 옷_x000D_
-ドスの気持ち</t>
+    <t>식재
+하플애플(ハップルアップル)
+푸기의 옷
+도스의 기분(ドスの気持ち)</t>
   </si>
   <si>
     <t>ドンドルマの道具屋の依頼2</t>
@@ -2544,8 +2538,8 @@
     <t>G★2 지보는 사과왕?(至宝の林檎王？)</t>
   </si>
   <si>
-    <t>식재_x000D_
-林檎王【凜護】</t>
+    <t>식재
+사과왕【름호】(林檎王【凜護】)</t>
   </si>
   <si>
     <t>船大工の親方の依頼</t>
@@ -2557,10 +2551,10 @@
     <t>집회소★6 가노토토스 모험기(ガノトトス冒険記)</t>
   </si>
   <si>
-    <t>식재_x000D_
-ブレスワイン
+    <t>식재
+브레스 와인(ブレスワイン)
 입수
-イカリハンマー</t>
+분노의 해머(イカリハンマー)</t>
   </si>
   <si>
     <t>シナト村の女の子の依頼</t>
@@ -2572,8 +2566,8 @@
     <t>마을★4 해앵사앙수해앵(행상수행)(ぎょーしょーしゅぎょー)</t>
   </si>
   <si>
-    <t>식재_x000D_
-完熟シナトマト</t>
+    <t>식재
+완숙 시나토 토마토(完熟シナトマト)</t>
   </si>
   <si>
     <t>まったりアイルーの依頼</t>
@@ -2585,10 +2579,10 @@
     <t>마을★5 빨간 해님 아뜨뜨(赤いおひさまアッチッチ)</t>
   </si>
   <si>
-    <t>식재_x000D_
-フワッフワッフル
+    <t>식재
+둥실둥실와플(フワッフワッフル)
 수기개방
-竜の息吹LV2</t>
+용의숨결LV2(竜の息吹LV2)</t>
   </si>
   <si>
     <t>ロックラックガイドの依頼</t>
@@ -2600,8 +2594,8 @@
     <t>마을★3 맛있는 알은 누구를 위해?(おいしい卵は誰のため？)</t>
   </si>
   <si>
-    <t>식재_x000D_
-ロックラッカセイ</t>
+    <t>식재
+록락 땅콩(ロックラッカセイ)</t>
   </si>
   <si>
     <t>タンジアの港のカシラの依頼</t>
@@ -2614,7 +2608,7 @@
   </si>
   <si>
     <t>장비개방
-ポルトマルク</t>
+폴트마르크(ポルトマルク)</t>
   </si>
   <si>
     <t>ギルドマネージャーの依頼</t>
@@ -2627,10 +2621,10 @@
   </si>
   <si>
     <t>장비개방
-番傘【秋雨】_x000D_
-アイリューシカ瓢弾
+지우산【추우】(番傘【秋雨】)
+아이류시카 표탄(アイリューシカ瓢弾)
 수기개방
-ブレイドダンスLV3</t>
+블레이드 댄스LV3(ブレイドダンスLV3)</t>
   </si>
   <si>
     <t>ミナガルデのご隠居の依頼</t>
@@ -2643,9 +2637,9 @@
   </si>
   <si>
     <t>장비개방
-大長老の脇差
+대장로의 작은 요도(大長老の脇差)
 수기개방
-バレットゲイザーLV3</t>
+블릿 게이저LV3(バレットゲイザーLV3)</t>
   </si>
   <si>
     <t>ロックラックの長の依頼1</t>
@@ -2658,9 +2652,9 @@
   </si>
   <si>
     <t>장비개방
-城塞遊撃隊/城塞弓撃隊シリーズ
+성채유격대/성채궁격대 시리즈(城塞遊撃隊/城塞弓撃隊シリーズ)
 수기개방
-獣宿し【餓狼】LV3</t>
+짐승깃들기【아랑】LV3(獣宿し【餓狼】LV3)</t>
   </si>
   <si>
     <t>ロックラックの長の依頼2</t>
@@ -2673,7 +2667,7 @@
   </si>
   <si>
     <t>장비개방
-城塞特攻隊/城塞隠密隊シリーズ</t>
+성채특공대/성채은밀대 시리즈(城塞特攻隊/城塞隠密隊シリーズ)</t>
   </si>
   <si>
     <t>モガの村の老職人の依頼1</t>
@@ -2686,9 +2680,9 @@
   </si>
   <si>
     <t>장비개방
-ヒーローアームズ_x000D_
-ヒーローガンランス_x000D_
-ヒーローブラスター</t>
+히어로 암즈(ヒーローアームズ)
+히어로 건랜스(ヒーローガンランス)
+히어로 블래스터(ヒーローブラスター)</t>
   </si>
   <si>
     <t>モガの村の老職人の依頼2</t>
@@ -2701,7 +2695,7 @@
   </si>
   <si>
     <t>퀘스트 보수
-大海原の輝石
+대해원의 휘석(大海原の輝石)
 장비개방
 ビクトリアーラ</t>
   </si>
@@ -2716,9 +2710,9 @@
   </si>
   <si>
     <t>오토모 장비개방
-マスターネコブレイド_x000D_
-マスターネコヘルム_x000D_
-マスターネコメイル</t>
+마스터 고양이 블레이드(マスターネコブレイド)
+마스터 고양이 헬름(マスターネコヘルム)
+마스터 고양이 메일(マスターネコメイル)</t>
   </si>
   <si>
     <t>그 외(その他)</t>
@@ -3251,8 +3245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C119" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="D179" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5403,7 +5397,7 @@
         <v>501</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>502</v>
+        <v>69</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30">
@@ -5411,16 +5405,16 @@
         <v>486</v>
       </c>
       <c r="B127" t="s">
+        <v>502</v>
+      </c>
+      <c r="C127" t="s">
         <v>503</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>504</v>
       </c>
-      <c r="D127" t="s">
+      <c r="E127" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="60">
@@ -5428,16 +5422,16 @@
         <v>486</v>
       </c>
       <c r="B128" t="s">
+        <v>506</v>
+      </c>
+      <c r="C128" t="s">
         <v>507</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>508</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" s="1" t="s">
         <v>509</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30">
@@ -5445,16 +5439,16 @@
         <v>486</v>
       </c>
       <c r="B129" t="s">
+        <v>510</v>
+      </c>
+      <c r="C129" t="s">
         <v>511</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
         <v>512</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" s="1" t="s">
         <v>513</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="90">
@@ -5462,16 +5456,16 @@
         <v>486</v>
       </c>
       <c r="B130" t="s">
+        <v>514</v>
+      </c>
+      <c r="C130" t="s">
         <v>515</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
         <v>516</v>
       </c>
-      <c r="D130" t="s">
+      <c r="E130" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="90">
@@ -5479,16 +5473,16 @@
         <v>486</v>
       </c>
       <c r="B131" t="s">
+        <v>518</v>
+      </c>
+      <c r="C131" t="s">
         <v>519</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
         <v>520</v>
       </c>
-      <c r="D131" t="s">
+      <c r="E131" s="1" t="s">
         <v>521</v>
-      </c>
-      <c r="E131" s="1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="75">
@@ -5496,16 +5490,16 @@
         <v>486</v>
       </c>
       <c r="B132" t="s">
+        <v>522</v>
+      </c>
+      <c r="C132" t="s">
         <v>523</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
         <v>524</v>
       </c>
-      <c r="D132" t="s">
+      <c r="E132" s="1" t="s">
         <v>525</v>
-      </c>
-      <c r="E132" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="75">
@@ -5513,16 +5507,16 @@
         <v>486</v>
       </c>
       <c r="B133" t="s">
+        <v>526</v>
+      </c>
+      <c r="C133" t="s">
         <v>527</v>
       </c>
-      <c r="C133" t="s">
+      <c r="D133" t="s">
         <v>528</v>
       </c>
-      <c r="D133" t="s">
+      <c r="E133" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="E133" s="1" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="30">
@@ -5530,16 +5524,16 @@
         <v>486</v>
       </c>
       <c r="B134" t="s">
+        <v>530</v>
+      </c>
+      <c r="C134" t="s">
         <v>531</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
         <v>532</v>
       </c>
-      <c r="D134" t="s">
+      <c r="E134" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="45">
@@ -5547,16 +5541,16 @@
         <v>486</v>
       </c>
       <c r="B135" t="s">
+        <v>534</v>
+      </c>
+      <c r="C135" t="s">
         <v>535</v>
       </c>
-      <c r="C135" t="s">
+      <c r="D135" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="45">
@@ -5564,16 +5558,16 @@
         <v>486</v>
       </c>
       <c r="B136" t="s">
+        <v>538</v>
+      </c>
+      <c r="C136" t="s">
         <v>539</v>
       </c>
-      <c r="C136" t="s">
+      <c r="D136" t="s">
         <v>540</v>
       </c>
-      <c r="D136" t="s">
+      <c r="E136" s="1" t="s">
         <v>541</v>
-      </c>
-      <c r="E136" s="1" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="45">
@@ -5581,16 +5575,16 @@
         <v>486</v>
       </c>
       <c r="B137" t="s">
+        <v>542</v>
+      </c>
+      <c r="C137" t="s">
         <v>543</v>
       </c>
-      <c r="C137" t="s">
+      <c r="D137" t="s">
         <v>544</v>
       </c>
-      <c r="D137" t="s">
+      <c r="E137" s="1" t="s">
         <v>545</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45">
@@ -5598,16 +5592,16 @@
         <v>486</v>
       </c>
       <c r="B138" t="s">
+        <v>546</v>
+      </c>
+      <c r="C138" t="s">
         <v>547</v>
       </c>
-      <c r="C138" t="s">
+      <c r="D138" t="s">
         <v>548</v>
       </c>
-      <c r="D138" t="s">
+      <c r="E138" s="1" t="s">
         <v>549</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="60">
@@ -5615,16 +5609,16 @@
         <v>486</v>
       </c>
       <c r="B139" t="s">
+        <v>550</v>
+      </c>
+      <c r="C139" t="s">
         <v>551</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
         <v>552</v>
       </c>
-      <c r="D139" t="s">
+      <c r="E139" s="1" t="s">
         <v>553</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="60">
@@ -5632,16 +5626,16 @@
         <v>486</v>
       </c>
       <c r="B140" t="s">
+        <v>554</v>
+      </c>
+      <c r="C140" t="s">
         <v>555</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
         <v>556</v>
       </c>
-      <c r="D140" t="s">
+      <c r="E140" s="1" t="s">
         <v>557</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="60">
@@ -5649,16 +5643,16 @@
         <v>486</v>
       </c>
       <c r="B141" t="s">
+        <v>558</v>
+      </c>
+      <c r="C141" t="s">
         <v>559</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>560</v>
       </c>
-      <c r="D141" t="s">
+      <c r="E141" s="1" t="s">
         <v>561</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30">
@@ -5666,16 +5660,16 @@
         <v>486</v>
       </c>
       <c r="B142" t="s">
+        <v>562</v>
+      </c>
+      <c r="C142" t="s">
         <v>563</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
         <v>564</v>
       </c>
-      <c r="D142" t="s">
+      <c r="E142" s="1" t="s">
         <v>565</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30">
@@ -5683,16 +5677,16 @@
         <v>486</v>
       </c>
       <c r="B143" t="s">
+        <v>566</v>
+      </c>
+      <c r="C143" t="s">
         <v>567</v>
       </c>
-      <c r="C143" t="s">
+      <c r="D143" t="s">
         <v>568</v>
       </c>
-      <c r="D143" t="s">
+      <c r="E143" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="E143" s="1" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30">
@@ -5700,16 +5694,16 @@
         <v>486</v>
       </c>
       <c r="B144" t="s">
+        <v>570</v>
+      </c>
+      <c r="C144" t="s">
         <v>571</v>
       </c>
-      <c r="C144" t="s">
+      <c r="D144" t="s">
         <v>572</v>
       </c>
-      <c r="D144" t="s">
+      <c r="E144" s="1" t="s">
         <v>573</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="30">
@@ -5717,16 +5711,16 @@
         <v>486</v>
       </c>
       <c r="B145" t="s">
+        <v>574</v>
+      </c>
+      <c r="C145" t="s">
         <v>575</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>576</v>
       </c>
-      <c r="D145" t="s">
+      <c r="E145" s="1" t="s">
         <v>577</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="30">
@@ -5734,16 +5728,16 @@
         <v>486</v>
       </c>
       <c r="B146" t="s">
+        <v>578</v>
+      </c>
+      <c r="C146" t="s">
         <v>579</v>
       </c>
-      <c r="C146" t="s">
+      <c r="D146" t="s">
         <v>580</v>
       </c>
-      <c r="D146" t="s">
+      <c r="E146" s="1" t="s">
         <v>581</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="30">
@@ -5751,16 +5745,16 @@
         <v>486</v>
       </c>
       <c r="B147" t="s">
+        <v>582</v>
+      </c>
+      <c r="C147" t="s">
         <v>583</v>
       </c>
-      <c r="C147" t="s">
+      <c r="D147" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="E147" s="1" t="s">
         <v>585</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="30">
@@ -5768,16 +5762,16 @@
         <v>486</v>
       </c>
       <c r="B148" t="s">
+        <v>586</v>
+      </c>
+      <c r="C148" t="s">
         <v>587</v>
       </c>
-      <c r="C148" t="s">
+      <c r="D148" t="s">
         <v>588</v>
       </c>
-      <c r="D148" t="s">
+      <c r="E148" s="1" t="s">
         <v>589</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="30">
@@ -5785,16 +5779,16 @@
         <v>486</v>
       </c>
       <c r="B149" t="s">
+        <v>590</v>
+      </c>
+      <c r="C149" t="s">
         <v>591</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>592</v>
       </c>
-      <c r="D149" t="s">
+      <c r="E149" s="1" t="s">
         <v>593</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30">
@@ -5802,16 +5796,16 @@
         <v>486</v>
       </c>
       <c r="B150" t="s">
+        <v>594</v>
+      </c>
+      <c r="C150" t="s">
         <v>595</v>
       </c>
-      <c r="C150" t="s">
+      <c r="D150" t="s">
         <v>596</v>
       </c>
-      <c r="D150" t="s">
+      <c r="E150" s="1" t="s">
         <v>597</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="90">
@@ -5819,16 +5813,16 @@
         <v>486</v>
       </c>
       <c r="B151" t="s">
+        <v>598</v>
+      </c>
+      <c r="C151" t="s">
         <v>599</v>
       </c>
-      <c r="C151" t="s">
+      <c r="D151" t="s">
         <v>600</v>
       </c>
-      <c r="D151" t="s">
+      <c r="E151" s="1" t="s">
         <v>601</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="45">
@@ -5836,16 +5830,16 @@
         <v>486</v>
       </c>
       <c r="B152" t="s">
+        <v>602</v>
+      </c>
+      <c r="C152" t="s">
         <v>603</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D152" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="D152" s="1" t="s">
+      <c r="E152" s="1" t="s">
         <v>605</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="30">
@@ -5853,16 +5847,16 @@
         <v>486</v>
       </c>
       <c r="B153" t="s">
+        <v>606</v>
+      </c>
+      <c r="C153" t="s">
         <v>607</v>
       </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>608</v>
       </c>
-      <c r="D153" t="s">
+      <c r="E153" s="1" t="s">
         <v>609</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5870,16 +5864,16 @@
         <v>486</v>
       </c>
       <c r="B154" t="s">
+        <v>610</v>
+      </c>
+      <c r="C154" t="s">
         <v>611</v>
       </c>
-      <c r="C154" t="s">
+      <c r="D154" t="s">
         <v>612</v>
       </c>
-      <c r="D154" t="s">
-        <v>613</v>
-      </c>
       <c r="E154" t="s">
-        <v>614</v>
+        <v>109</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="75">
@@ -5887,16 +5881,16 @@
         <v>486</v>
       </c>
       <c r="B155" t="s">
+        <v>613</v>
+      </c>
+      <c r="C155" t="s">
+        <v>614</v>
+      </c>
+      <c r="D155" t="s">
         <v>615</v>
       </c>
-      <c r="C155" t="s">
+      <c r="E155" s="1" t="s">
         <v>616</v>
-      </c>
-      <c r="D155" t="s">
-        <v>617</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="75">
@@ -5904,16 +5898,16 @@
         <v>486</v>
       </c>
       <c r="B156" t="s">
+        <v>617</v>
+      </c>
+      <c r="C156" t="s">
+        <v>618</v>
+      </c>
+      <c r="D156" t="s">
         <v>619</v>
       </c>
-      <c r="C156" t="s">
+      <c r="E156" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="D156" t="s">
-        <v>621</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="75">
@@ -5921,16 +5915,16 @@
         <v>486</v>
       </c>
       <c r="B157" t="s">
+        <v>621</v>
+      </c>
+      <c r="C157" t="s">
+        <v>622</v>
+      </c>
+      <c r="D157" t="s">
         <v>623</v>
       </c>
-      <c r="C157" t="s">
+      <c r="E157" s="1" t="s">
         <v>624</v>
-      </c>
-      <c r="D157" t="s">
-        <v>625</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5938,33 +5932,33 @@
         <v>486</v>
       </c>
       <c r="B158" t="s">
+        <v>625</v>
+      </c>
+      <c r="C158" t="s">
+        <v>626</v>
+      </c>
+      <c r="D158" t="s">
         <v>627</v>
       </c>
-      <c r="C158" t="s">
-        <v>628</v>
-      </c>
-      <c r="D158" t="s">
-        <v>629</v>
-      </c>
       <c r="E158" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" ht="60">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="75">
       <c r="A159" t="s">
         <v>486</v>
       </c>
       <c r="B159" t="s">
+        <v>628</v>
+      </c>
+      <c r="C159" t="s">
+        <v>629</v>
+      </c>
+      <c r="D159" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="C159" t="s">
+      <c r="E159" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="E159" s="1" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="30">
@@ -5972,16 +5966,16 @@
         <v>486</v>
       </c>
       <c r="B160" t="s">
+        <v>632</v>
+      </c>
+      <c r="C160" t="s">
+        <v>633</v>
+      </c>
+      <c r="D160" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="C160" t="s">
+      <c r="E160" s="1" t="s">
         <v>635</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="30">
@@ -5989,16 +5983,16 @@
         <v>486</v>
       </c>
       <c r="B161" t="s">
+        <v>636</v>
+      </c>
+      <c r="C161" t="s">
+        <v>637</v>
+      </c>
+      <c r="D161" t="s">
         <v>638</v>
       </c>
-      <c r="C161" t="s">
+      <c r="E161" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="D161" t="s">
-        <v>640</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="30">
@@ -6006,16 +6000,16 @@
         <v>486</v>
       </c>
       <c r="B162" t="s">
+        <v>640</v>
+      </c>
+      <c r="C162" t="s">
+        <v>641</v>
+      </c>
+      <c r="D162" t="s">
         <v>642</v>
       </c>
-      <c r="C162" t="s">
+      <c r="E162" s="1" t="s">
         <v>643</v>
-      </c>
-      <c r="D162" t="s">
-        <v>644</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -6023,16 +6017,16 @@
         <v>486</v>
       </c>
       <c r="B163" t="s">
+        <v>644</v>
+      </c>
+      <c r="C163" t="s">
+        <v>645</v>
+      </c>
+      <c r="D163" t="s">
         <v>646</v>
       </c>
-      <c r="C163" t="s">
-        <v>647</v>
-      </c>
-      <c r="D163" t="s">
-        <v>648</v>
-      </c>
       <c r="E163" t="s">
-        <v>614</v>
+        <v>109</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="30">
@@ -6040,16 +6034,16 @@
         <v>486</v>
       </c>
       <c r="B164" t="s">
+        <v>647</v>
+      </c>
+      <c r="C164" t="s">
+        <v>648</v>
+      </c>
+      <c r="D164" t="s">
         <v>649</v>
       </c>
-      <c r="C164" t="s">
+      <c r="E164" s="1" t="s">
         <v>650</v>
-      </c>
-      <c r="D164" t="s">
-        <v>651</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="60">
@@ -6057,16 +6051,16 @@
         <v>486</v>
       </c>
       <c r="B165" t="s">
+        <v>651</v>
+      </c>
+      <c r="C165" t="s">
+        <v>652</v>
+      </c>
+      <c r="D165" t="s">
         <v>653</v>
       </c>
-      <c r="C165" t="s">
+      <c r="E165" s="1" t="s">
         <v>654</v>
-      </c>
-      <c r="D165" t="s">
-        <v>655</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="60">
@@ -6074,16 +6068,16 @@
         <v>486</v>
       </c>
       <c r="B166" t="s">
+        <v>655</v>
+      </c>
+      <c r="C166" t="s">
+        <v>656</v>
+      </c>
+      <c r="D166" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="C166" t="s">
+      <c r="E166" s="1" t="s">
         <v>658</v>
-      </c>
-      <c r="D166" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="E166" s="1" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="30">
@@ -6091,16 +6085,16 @@
         <v>486</v>
       </c>
       <c r="B167" t="s">
+        <v>659</v>
+      </c>
+      <c r="C167" t="s">
+        <v>660</v>
+      </c>
+      <c r="D167" t="s">
         <v>661</v>
       </c>
-      <c r="C167" t="s">
+      <c r="E167" s="1" t="s">
         <v>662</v>
-      </c>
-      <c r="D167" t="s">
-        <v>663</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="30">
@@ -6108,16 +6102,16 @@
         <v>486</v>
       </c>
       <c r="B168" t="s">
+        <v>663</v>
+      </c>
+      <c r="C168" t="s">
+        <v>664</v>
+      </c>
+      <c r="D168" t="s">
         <v>665</v>
       </c>
-      <c r="C168" t="s">
+      <c r="E168" s="1" t="s">
         <v>666</v>
-      </c>
-      <c r="D168" t="s">
-        <v>667</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="169" spans="1:5" ht="30">
@@ -6125,16 +6119,16 @@
         <v>486</v>
       </c>
       <c r="B169" t="s">
+        <v>667</v>
+      </c>
+      <c r="C169" t="s">
+        <v>668</v>
+      </c>
+      <c r="D169" t="s">
         <v>669</v>
       </c>
-      <c r="C169" t="s">
+      <c r="E169" s="1" t="s">
         <v>670</v>
-      </c>
-      <c r="D169" t="s">
-        <v>671</v>
-      </c>
-      <c r="E169" s="1" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="60">
@@ -6142,16 +6136,16 @@
         <v>486</v>
       </c>
       <c r="B170" t="s">
+        <v>671</v>
+      </c>
+      <c r="C170" t="s">
+        <v>672</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>673</v>
       </c>
-      <c r="C170" t="s">
+      <c r="E170" s="1" t="s">
         <v>674</v>
-      </c>
-      <c r="D170" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="60">
@@ -6159,16 +6153,16 @@
         <v>486</v>
       </c>
       <c r="B171" t="s">
+        <v>675</v>
+      </c>
+      <c r="C171" t="s">
+        <v>676</v>
+      </c>
+      <c r="D171" t="s">
         <v>677</v>
       </c>
-      <c r="C171" t="s">
+      <c r="E171" s="1" t="s">
         <v>678</v>
-      </c>
-      <c r="D171" t="s">
-        <v>679</v>
-      </c>
-      <c r="E171" s="1" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="30">
@@ -6176,16 +6170,16 @@
         <v>486</v>
       </c>
       <c r="B172" t="s">
+        <v>679</v>
+      </c>
+      <c r="C172" t="s">
+        <v>680</v>
+      </c>
+      <c r="D172" t="s">
         <v>681</v>
       </c>
-      <c r="C172" t="s">
+      <c r="E172" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="D172" t="s">
-        <v>683</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="60">
@@ -6193,16 +6187,16 @@
         <v>486</v>
       </c>
       <c r="B173" t="s">
+        <v>683</v>
+      </c>
+      <c r="C173" t="s">
+        <v>684</v>
+      </c>
+      <c r="D173" t="s">
         <v>685</v>
       </c>
-      <c r="C173" t="s">
+      <c r="E173" s="1" t="s">
         <v>686</v>
-      </c>
-      <c r="D173" t="s">
-        <v>687</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="174" spans="1:5" ht="30">
@@ -6210,16 +6204,16 @@
         <v>486</v>
       </c>
       <c r="B174" t="s">
+        <v>687</v>
+      </c>
+      <c r="C174" t="s">
+        <v>688</v>
+      </c>
+      <c r="D174" t="s">
         <v>689</v>
       </c>
-      <c r="C174" t="s">
+      <c r="E174" s="1" t="s">
         <v>690</v>
-      </c>
-      <c r="D174" t="s">
-        <v>691</v>
-      </c>
-      <c r="E174" s="1" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="60">
@@ -6227,16 +6221,16 @@
         <v>486</v>
       </c>
       <c r="B175" t="s">
+        <v>691</v>
+      </c>
+      <c r="C175" t="s">
+        <v>692</v>
+      </c>
+      <c r="D175" t="s">
         <v>693</v>
       </c>
-      <c r="C175" t="s">
+      <c r="E175" s="1" t="s">
         <v>694</v>
-      </c>
-      <c r="D175" t="s">
-        <v>695</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="176" spans="1:5" ht="30">
@@ -6244,16 +6238,16 @@
         <v>486</v>
       </c>
       <c r="B176" t="s">
+        <v>695</v>
+      </c>
+      <c r="C176" t="s">
+        <v>696</v>
+      </c>
+      <c r="D176" t="s">
         <v>697</v>
       </c>
-      <c r="C176" t="s">
+      <c r="E176" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="D176" t="s">
-        <v>699</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="177" spans="1:5" ht="30">
@@ -6261,16 +6255,16 @@
         <v>486</v>
       </c>
       <c r="B177" t="s">
+        <v>699</v>
+      </c>
+      <c r="C177" t="s">
+        <v>700</v>
+      </c>
+      <c r="D177" t="s">
         <v>701</v>
       </c>
-      <c r="C177" t="s">
+      <c r="E177" s="1" t="s">
         <v>702</v>
-      </c>
-      <c r="D177" t="s">
-        <v>703</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="178" spans="1:5" ht="75">
@@ -6278,16 +6272,16 @@
         <v>486</v>
       </c>
       <c r="B178" t="s">
+        <v>703</v>
+      </c>
+      <c r="C178" t="s">
+        <v>704</v>
+      </c>
+      <c r="D178" t="s">
         <v>705</v>
       </c>
-      <c r="C178" t="s">
+      <c r="E178" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="D178" t="s">
-        <v>707</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="179" spans="1:5" ht="60">
@@ -6295,16 +6289,16 @@
         <v>486</v>
       </c>
       <c r="B179" t="s">
+        <v>707</v>
+      </c>
+      <c r="C179" t="s">
+        <v>708</v>
+      </c>
+      <c r="D179" t="s">
         <v>709</v>
       </c>
-      <c r="C179" t="s">
+      <c r="E179" s="1" t="s">
         <v>710</v>
-      </c>
-      <c r="D179" t="s">
-        <v>711</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="180" spans="1:5" ht="60">
@@ -6312,16 +6306,16 @@
         <v>486</v>
       </c>
       <c r="B180" t="s">
+        <v>711</v>
+      </c>
+      <c r="C180" t="s">
+        <v>712</v>
+      </c>
+      <c r="D180" t="s">
         <v>713</v>
       </c>
-      <c r="C180" t="s">
+      <c r="E180" s="1" t="s">
         <v>714</v>
-      </c>
-      <c r="D180" t="s">
-        <v>715</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="181" spans="1:5" ht="30">
@@ -6329,16 +6323,16 @@
         <v>486</v>
       </c>
       <c r="B181" t="s">
+        <v>715</v>
+      </c>
+      <c r="C181" t="s">
+        <v>716</v>
+      </c>
+      <c r="D181" t="s">
         <v>717</v>
       </c>
-      <c r="C181" t="s">
+      <c r="E181" s="1" t="s">
         <v>718</v>
-      </c>
-      <c r="D181" t="s">
-        <v>719</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="182" spans="1:5" ht="60">
@@ -6346,16 +6340,16 @@
         <v>486</v>
       </c>
       <c r="B182" t="s">
+        <v>719</v>
+      </c>
+      <c r="C182" t="s">
+        <v>720</v>
+      </c>
+      <c r="D182" t="s">
         <v>721</v>
       </c>
-      <c r="C182" t="s">
+      <c r="E182" s="1" t="s">
         <v>722</v>
-      </c>
-      <c r="D182" t="s">
-        <v>723</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="183" spans="1:5" ht="60">
@@ -6363,16 +6357,16 @@
         <v>486</v>
       </c>
       <c r="B183" t="s">
+        <v>723</v>
+      </c>
+      <c r="C183" t="s">
+        <v>724</v>
+      </c>
+      <c r="D183" t="s">
         <v>725</v>
       </c>
-      <c r="C183" t="s">
+      <c r="E183" s="1" t="s">
         <v>726</v>
-      </c>
-      <c r="D183" t="s">
-        <v>727</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="184" spans="1:5" ht="60">
@@ -6380,203 +6374,203 @@
         <v>486</v>
       </c>
       <c r="B184" t="s">
+        <v>727</v>
+      </c>
+      <c r="C184" t="s">
+        <v>728</v>
+      </c>
+      <c r="D184" t="s">
         <v>729</v>
       </c>
-      <c r="C184" t="s">
+      <c r="E184" s="1" t="s">
         <v>730</v>
-      </c>
-      <c r="D184" t="s">
-        <v>731</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="30">
       <c r="A185" t="s">
+        <v>731</v>
+      </c>
+      <c r="B185" t="s">
+        <v>732</v>
+      </c>
+      <c r="C185" t="s">
         <v>733</v>
       </c>
-      <c r="B185" t="s">
+      <c r="D185" t="s">
         <v>734</v>
       </c>
-      <c r="C185" t="s">
+      <c r="E185" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="D185" t="s">
-        <v>736</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="186" spans="1:5" ht="30">
       <c r="A186" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B186" t="s">
+        <v>736</v>
+      </c>
+      <c r="C186" t="s">
+        <v>737</v>
+      </c>
+      <c r="D186" t="s">
         <v>738</v>
       </c>
-      <c r="C186" t="s">
+      <c r="E186" s="1" t="s">
         <v>739</v>
-      </c>
-      <c r="D186" t="s">
-        <v>740</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="30">
       <c r="A187" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B187" t="s">
+        <v>740</v>
+      </c>
+      <c r="C187" t="s">
+        <v>741</v>
+      </c>
+      <c r="D187" t="s">
         <v>742</v>
       </c>
-      <c r="C187" t="s">
+      <c r="E187" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="D187" t="s">
-        <v>744</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="30">
       <c r="A188" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B188" t="s">
+        <v>744</v>
+      </c>
+      <c r="C188" t="s">
+        <v>745</v>
+      </c>
+      <c r="D188" t="s">
         <v>746</v>
       </c>
-      <c r="C188" t="s">
+      <c r="E188" s="1" t="s">
         <v>747</v>
-      </c>
-      <c r="D188" t="s">
-        <v>748</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="189" spans="1:5" ht="30">
       <c r="A189" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B189" t="s">
+        <v>748</v>
+      </c>
+      <c r="C189" t="s">
+        <v>749</v>
+      </c>
+      <c r="D189" t="s">
         <v>750</v>
       </c>
-      <c r="C189" t="s">
+      <c r="E189" s="1" t="s">
         <v>751</v>
-      </c>
-      <c r="D189" t="s">
-        <v>752</v>
-      </c>
-      <c r="E189" s="1" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="190" spans="1:5" ht="30">
       <c r="A190" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B190" t="s">
+        <v>752</v>
+      </c>
+      <c r="C190" t="s">
+        <v>753</v>
+      </c>
+      <c r="D190" t="s">
         <v>754</v>
       </c>
-      <c r="C190" t="s">
+      <c r="E190" s="1" t="s">
         <v>755</v>
-      </c>
-      <c r="D190" t="s">
-        <v>756</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="191" spans="1:5" ht="30">
       <c r="A191" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B191" t="s">
+        <v>756</v>
+      </c>
+      <c r="C191" t="s">
+        <v>757</v>
+      </c>
+      <c r="D191" t="s">
         <v>758</v>
       </c>
-      <c r="C191" t="s">
+      <c r="E191" s="1" t="s">
         <v>759</v>
-      </c>
-      <c r="D191" t="s">
-        <v>760</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="30">
       <c r="A192" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B192" t="s">
+        <v>760</v>
+      </c>
+      <c r="C192" t="s">
+        <v>761</v>
+      </c>
+      <c r="D192" t="s">
         <v>762</v>
       </c>
-      <c r="C192" t="s">
+      <c r="E192" s="1" t="s">
         <v>763</v>
-      </c>
-      <c r="D192" t="s">
-        <v>764</v>
-      </c>
-      <c r="E192" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="30">
       <c r="A193" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B193" t="s">
+        <v>764</v>
+      </c>
+      <c r="C193" t="s">
+        <v>765</v>
+      </c>
+      <c r="D193" t="s">
         <v>766</v>
       </c>
-      <c r="C193" t="s">
+      <c r="E193" s="1" t="s">
         <v>767</v>
-      </c>
-      <c r="D193" t="s">
-        <v>768</v>
-      </c>
-      <c r="E193" s="1" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="45">
       <c r="A194" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B194" t="s">
+        <v>768</v>
+      </c>
+      <c r="C194" t="s">
+        <v>769</v>
+      </c>
+      <c r="D194" t="s">
         <v>770</v>
       </c>
-      <c r="C194" t="s">
+      <c r="E194" s="1" t="s">
         <v>771</v>
-      </c>
-      <c r="D194" t="s">
-        <v>772</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="90">
       <c r="A195" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B195" t="s">
+        <v>772</v>
+      </c>
+      <c r="C195" t="s">
+        <v>773</v>
+      </c>
+      <c r="D195" t="s">
         <v>774</v>
       </c>
-      <c r="C195" t="s">
+      <c r="E195" s="1" t="s">
         <v>775</v>
-      </c>
-      <c r="D195" t="s">
-        <v>776</v>
-      </c>
-      <c r="E195" s="1" t="s">
-        <v>777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
requestQuest: Name translation of equipment and foodstuffs to be opened.(~End)
</commit_message>
<xml_diff>
--- a/request.xlsx
+++ b/request.xlsx
@@ -2728,7 +2728,7 @@
   </si>
   <si>
     <t>입수
-鶴寿の羽飾り</t>
+학수의 깃털 장식(鶴寿の羽飾り)</t>
   </si>
   <si>
     <t>その他2</t>
@@ -2741,7 +2741,7 @@
   </si>
   <si>
     <t>입수
-剣聖のピアス</t>
+검성의 피어스(剣聖のピアス)</t>
   </si>
   <si>
     <t>その他3</t>
@@ -2754,7 +2754,7 @@
   </si>
   <si>
     <t>입수
-増弾のピアス</t>
+증탄의 피어스(増弾のピアス)</t>
   </si>
   <si>
     <t>その他4</t>
@@ -2767,7 +2767,7 @@
   </si>
   <si>
     <t>입수
-虚心のピアス</t>
+허심의 피어스(虚心のピアス)</t>
   </si>
   <si>
     <t>その他5</t>
@@ -2780,7 +2780,7 @@
   </si>
   <si>
     <t>입수
-切望のピアス</t>
+절망의 피어스(切望のピアス)</t>
   </si>
   <si>
     <t>その他6</t>
@@ -2793,7 +2793,7 @@
   </si>
   <si>
     <t>입수
-ベルナ・フィオーレ</t>
+베르나・피오레(ベルナ・フィオーレ)</t>
   </si>
   <si>
     <t>その他7</t>
@@ -2806,7 +2806,7 @@
   </si>
   <si>
     <t>입수
-ココット・アルベロ</t>
+코코트・알베로(ココット・アルベロ)</t>
   </si>
   <si>
     <t>その他8</t>
@@ -2819,7 +2819,7 @@
   </si>
   <si>
     <t>입수
-ポッケ・ネーヴェ</t>
+폿케・네베(ポッケ・ネーヴェ)</t>
   </si>
   <si>
     <t>その他9</t>
@@ -2832,7 +2832,7 @@
   </si>
   <si>
     <t>입수
-ユクモ・テルメ</t>
+유쿠모・테르메(ユクモ・テルメ)</t>
   </si>
   <si>
     <t>その他10</t>
@@ -2845,8 +2845,8 @@
   </si>
   <si>
     <t>입수
-セーリオシリーズ_x000D_
-シャルマンシリーズ</t>
+세리오 시리즈(セーリオシリーズ)
+샬만 시리즈(シャルマンシリーズ)</t>
   </si>
   <si>
     <t>その他11</t>
@@ -2859,11 +2859,11 @@
   </si>
   <si>
     <t>입수
-斬炎のピアス_x000D_
-雷電のピアス_x000D_
-巨氷のピアス_x000D_
-水狐のピアス_x000D_
-龍彗のピアス</t>
+참염의 피어스(斬炎のピアス)
+뇌전의 피어스(雷電のピアス)
+거빙의 피어스(巨氷のピアス)
+수호의 피어스(水狐のピアス)
+용혜의 피어스(龍彗のピアス)</t>
   </si>
 </sst>
 </file>
@@ -3245,8 +3245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D179" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="D185" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>